<commit_message>
massive redesign of obs units
</commit_message>
<xml_diff>
--- a/NelsonLab Online Database Dictionary.xlsx
+++ b/NelsonLab Online Database Dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\RNelson Lab\RJNelson Lab Handbook\Database information\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Documents\GitHub\django_NelsonDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1767,8 +1767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A240" workbookViewId="0">
-      <selection activeCell="C266" sqref="C266"/>
+    <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
+      <selection activeCell="C246" sqref="C246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4238,7 +4238,7 @@
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B247" t="s">
         <v>14</v>
@@ -4249,7 +4249,7 @@
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B248" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
change to obstracker by adding obstrackersource
</commit_message>
<xml_diff>
--- a/NelsonLab Online Database Dictionary.xlsx
+++ b/NelsonLab Online Database Dictionary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="400">
   <si>
     <t>NelsonLab Online Database Dictionary</t>
   </si>
@@ -327,12 +327,6 @@
     <t xml:space="preserve">The user's position or title. </t>
   </si>
   <si>
-    <t>lab_ObsSelector</t>
-  </si>
-  <si>
-    <t>The experiment to which the data is linked to. This is specifically the id in lab_experiment. It is generally selected using the experiment name because the name is unique: experiment_id = Experiment(name).id</t>
-  </si>
-  <si>
     <t>lab_ObsRow</t>
   </si>
   <si>
@@ -367,12 +361,6 @@
   </si>
   <si>
     <t>harvest_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is the observation's unique obs_selector_id. This is specifically the id from lab_ObsSelector. </t>
-  </si>
-  <si>
-    <t>The field in which the row was planted in. Specifically, this is the id from lab_field. Generally this is selected using the field name because the field name is unique: field_id = Field(field_name).id</t>
   </si>
   <si>
     <r>
@@ -436,9 +424,6 @@
     <t>plant_id</t>
   </si>
   <si>
-    <t>This is the seed stock which was planted in the row. Specifically it is the id for lab_stock. Generally it is selected using the seed_id because the seed_id is unique: stock_id = Stock(seed_id).id</t>
-  </si>
-  <si>
     <t>The plant's number assignment.</t>
   </si>
   <si>
@@ -458,12 +443,6 @@
     </r>
   </si>
   <si>
-    <t>The row in which the plant was grown. Specifically this is the id in lab_ObsRow. Generally selected using the row id because the row_id is unique: obs_row_id = ObsRow(row_id).id</t>
-  </si>
-  <si>
-    <t>The seed stock which the plant was planted from. Specifically this is the id from lab_stock. Generally selected using the seed id because seed ids are unique: stock_id = Stock(seed_id).id</t>
-  </si>
-  <si>
     <t>lab_ObsEnv</t>
   </si>
   <si>
@@ -483,9 +462,6 @@
   </si>
   <si>
     <t>Any additional comments about the plant.</t>
-  </si>
-  <si>
-    <t>The field in which the environment is. This is specifically  the id from lab_field. It is generally selected using the field name because the field name is unique: field_id = Field(field_name).id</t>
   </si>
   <si>
     <r>
@@ -510,72 +486,15 @@
     <t>The latitude coordinate of the environment.</t>
   </si>
   <si>
-    <t>lab_ObsOther</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This table holds a variety of distinct entity types. It is similar to the ObsRow, ObsPlant, and ObsEnv tables above, but it is different in that if does not hold data only for a single entity. This table is analogous to a combination of ObsDNA, ObsTissue, ObsPlate, ObsSample, ObsWell, ObsCulture, and ObsMicrobe tables.It would be possible to merge ObsRow, ObsPlant, and ObsEnv into this table, but for performance and legacy reasons, those entity types will be left distinct. This table includes a variety of source fields to accomodate any combination: For example, if DNA was isolated from tissues, it would haave a source_tissue_id. </t>
-  </si>
-  <si>
     <t>medium_id</t>
   </si>
   <si>
     <t>location_id</t>
   </si>
   <si>
-    <t>source_stock_id</t>
-  </si>
-  <si>
-    <t>source_isolate_id</t>
-  </si>
-  <si>
-    <t>source_row_id</t>
-  </si>
-  <si>
-    <t>source_plant_id</t>
-  </si>
-  <si>
-    <t>source_well_id</t>
-  </si>
-  <si>
-    <t>source_microbe_id</t>
-  </si>
-  <si>
-    <t>source_culture_id</t>
-  </si>
-  <si>
-    <t>source_tissue_id</t>
-  </si>
-  <si>
-    <t>source_sample_id</t>
-  </si>
-  <si>
-    <t>source_dna_id</t>
-  </si>
-  <si>
-    <t>source_plate_id</t>
-  </si>
-  <si>
-    <t>entity_type</t>
-  </si>
-  <si>
     <t>dna_id</t>
   </si>
   <si>
-    <t>dna_extraction_method</t>
-  </si>
-  <si>
-    <t>dna_date</t>
-  </si>
-  <si>
-    <t>dna_tube_id</t>
-  </si>
-  <si>
-    <t>dna_tube_type</t>
-  </si>
-  <si>
-    <t>dna_comments</t>
-  </si>
-  <si>
     <t>tissue_id</t>
   </si>
   <si>
@@ -585,139 +504,40 @@
     <t>tissue_name</t>
   </si>
   <si>
-    <t>tissue_date_ground</t>
-  </si>
-  <si>
-    <t>tissue_comments</t>
-  </si>
-  <si>
     <t>plate_id</t>
   </si>
   <si>
     <t>plate_name</t>
   </si>
   <si>
-    <t>plate_date_plated</t>
-  </si>
-  <si>
-    <t>plate_contents</t>
-  </si>
-  <si>
-    <t>plate_rep</t>
-  </si>
-  <si>
     <t>plate_type</t>
   </si>
   <si>
     <t>plate_status</t>
   </si>
   <si>
-    <t>plate_comments</t>
-  </si>
-  <si>
     <t>sample_id</t>
   </si>
   <si>
     <t>sample_type</t>
   </si>
   <si>
-    <t>sample_weight</t>
-  </si>
-  <si>
-    <t>sample_kernel_num</t>
-  </si>
-  <si>
-    <t>sample_comments</t>
-  </si>
-  <si>
     <t>well_id</t>
   </si>
   <si>
     <t>well_inventory</t>
   </si>
   <si>
-    <t>well</t>
-  </si>
-  <si>
-    <t>well_tube_label</t>
-  </si>
-  <si>
-    <t>well_comments</t>
-  </si>
-  <si>
     <t>culture_id</t>
   </si>
   <si>
     <t>culture_name</t>
   </si>
   <si>
-    <t>culture_microbe_type</t>
-  </si>
-  <si>
-    <t>culture_plating_cycle</t>
-  </si>
-  <si>
-    <t>culture_dilution</t>
-  </si>
-  <si>
-    <t>culture_image</t>
-  </si>
-  <si>
-    <t>culture_comments</t>
-  </si>
-  <si>
     <t>microbe_id</t>
   </si>
   <si>
     <t>microbe_type</t>
-  </si>
-  <si>
-    <t>microbe_comments</t>
-  </si>
-  <si>
-    <t>The user which is responsible for creating the entity. Specifically this is the is from auth_user. Usernames are used to select this because usernames are unique: user_id = User(username).id</t>
-  </si>
-  <si>
-    <t>The medium that was used to grow the entity. Generally this is only relevant to cultures. Specifically this is the id from lab_medium. Media Type is used to select this because media types are unique: medium_id = Medium(media_type).id</t>
-  </si>
-  <si>
-    <t>The location for the entity. Specifically this is the id from lab_location. Location names are used to select this because location names are unique: location_id = Location(location_name).id</t>
-  </si>
-  <si>
-    <t>For if the entity was from a specific isolate. Specifically this is the id from lab_isolate. Isolate IDs are used to select this because isolate IDs are unique: source_isolate_id = Isolate(isolate_id).id</t>
-  </si>
-  <si>
-    <t>For if the entity is associated to a seed_id, such as if DNA was isolated from seed. Specifically this is the id from lab_stock. Seed IDs are used to select this because seed IDs are unique: source_stock_id = Stock(seed_id).id</t>
-  </si>
-  <si>
-    <t>For if the entity was from a specific row. Specifically this is the id from lab_ObsRow. Row IDs are used to select this because row IDs are unique: source_row_id = ObsRow(row_id).id</t>
-  </si>
-  <si>
-    <t>For if the entity was from a specific plant. Specifically this the id from ObsOther, pointing recursvicely. Plant IDs are used to select this because plant IDs are unique: source_plant_id = ObsOther(plant_id).id</t>
-  </si>
-  <si>
-    <t>For if the entity was from a specific well. Specifically this the id from ObsOther, pointing recursvicely. Well IDs are used to select this because well IDs are unique: source_well_id = ObsOther(well_id).id</t>
-  </si>
-  <si>
-    <t>For if the entity was from a specific microbe. Specifically this the id from ObsOther, pointing recursvicely. Microbe IDs are used to select this because microbe IDs are unique: source_microbe_id = ObsOther(microbe_id).id</t>
-  </si>
-  <si>
-    <t>For if the entity was from a specific culture. Specifically this the id from ObsOther, pointing recursvicely. Culture IDs are used to select this because culture IDs are unique: source_culture_id = ObsOther(culture_id).id</t>
-  </si>
-  <si>
-    <t>For if the entity was from a specific tissue. Specifically this the id from ObsOther, pointing recursvicely. Tissue IDs are used to select this because tissue IDs are unique: source_tissue_id = ObsOther(tissue_id).id</t>
-  </si>
-  <si>
-    <t>For if the entity was from a specific sample. Specifically this the id from ObsOther, pointing recursvicely. Sample IDs are used to select this because sample IDs are unique: source_sample_id = ObsOther(sample_id).id</t>
-  </si>
-  <si>
-    <t>For if the entity was from a specific dna. Specifically this the id from ObsOther, pointing recursvicely. Dna IDs are used to select this because dna IDs are unique: source_dna_id = ObsOther(dna_id).id</t>
-  </si>
-  <si>
-    <t>For if the entity was from a specific plate. Specifically this the id from ObsOther, pointing recursvicely. Plate IDs are used to select this because plate IDs are unique: source_plate_id = ObsOther(plate_id).id</t>
-  </si>
-  <si>
-    <t>The type of entity being recorded. Either Tissue, DNA, Plate, Sample, Culture, Well, or Microbe</t>
   </si>
   <si>
     <r>
@@ -1251,9 +1071,6 @@
     <t>Any additional comments about the source or person.</t>
   </si>
   <si>
-    <t>This table allows different observation unit types to be connected to the measurement table, experiment table, and collecting table. Observation unit types are stored in four tables currently: ObsRow, ObsPlant, ObsEnv, and ObsOther (holds Plate, Culture, Well, DNA, Tissue, Samples, and Microbe types). While these four tables could be condensed into one massive table, in the same manner as ObsOther, it is more useful to keep them separate for performance and legacy purposes. Every observation unit is assigned a unique autoincrementing integer known as the obs_selector_id, in order to assure that all observation units have a unique id.</t>
-  </si>
-  <si>
     <t>An automatically assigned, unique, auto-increment integer. Example: 1,2,3,4,5…</t>
   </si>
   <si>
@@ -1386,6 +1203,287 @@
   </si>
   <si>
     <t xml:space="preserve">Holds info for all diseases dealt with in the lab. </t>
+  </si>
+  <si>
+    <t>lab_Citation</t>
+  </si>
+  <si>
+    <t>Any citations are stored here. Currently only the Medium table uses citations.</t>
+  </si>
+  <si>
+    <t>citation_type</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>pubmed_id</t>
+  </si>
+  <si>
+    <t>The type of citation. Example: Literature, Online Journal, Textbook</t>
+  </si>
+  <si>
+    <t>The online URL to the article or resource.</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A unique title for the citation. It can be the title of the article or resource. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MUST BE UNIQUE</t>
+    </r>
+  </si>
+  <si>
+    <t>The unique Pubmed ID. If not appplicable, leave blank.</t>
+  </si>
+  <si>
+    <t>Any additional comments about the citation.</t>
+  </si>
+  <si>
+    <t>lab_Medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Any media that is used in the lab is stored here. </t>
+  </si>
+  <si>
+    <t>media_name</t>
+  </si>
+  <si>
+    <t>media_type</t>
+  </si>
+  <si>
+    <t>media_description</t>
+  </si>
+  <si>
+    <t>media_preparation</t>
+  </si>
+  <si>
+    <t>The relevant citation for the media. Specifically this the id from lab_medium. Citation titles are used to select this because titles are unique: citation= Citation(title).id</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A unique name for the media. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MUST BE UNIQUE</t>
+    </r>
+  </si>
+  <si>
+    <t>The type of media being used. Example: Bacterial, Fungal</t>
+  </si>
+  <si>
+    <t>A brief description of the media, including any inhibiting or growth effects.</t>
+  </si>
+  <si>
+    <t>A brief description of how to prepare the media.</t>
+  </si>
+  <si>
+    <t>Any additional comments about the medium.</t>
+  </si>
+  <si>
+    <t>obs_tracker_id</t>
+  </si>
+  <si>
+    <t>This is the observation's unique obs_tracker_id. The obs_tracker_id links all the various obs data types to measurements, experiments, as well as any dependencies such as seed stocks.</t>
+  </si>
+  <si>
+    <t>lab_ObsDNA</t>
+  </si>
+  <si>
+    <t>extraction_method</t>
+  </si>
+  <si>
+    <t>tube_id</t>
+  </si>
+  <si>
+    <t>tube_type</t>
+  </si>
+  <si>
+    <t>lab_ObsMicrobe</t>
+  </si>
+  <si>
+    <t>lab_ObsCulture</t>
+  </si>
+  <si>
+    <t>plating_cycle</t>
+  </si>
+  <si>
+    <t>dilution</t>
+  </si>
+  <si>
+    <t>image_filename</t>
+  </si>
+  <si>
+    <t>lab_ObsSample</t>
+  </si>
+  <si>
+    <t>lab_ObsTissue</t>
+  </si>
+  <si>
+    <t>date_ground</t>
+  </si>
+  <si>
+    <t>lab_ObsWell</t>
+  </si>
+  <si>
+    <t>tube_label</t>
+  </si>
+  <si>
+    <t>lab_ObsPlate</t>
+  </si>
+  <si>
+    <t>contents</t>
+  </si>
+  <si>
+    <t>This table holds any DNA extracts that need to be recorded. This information is for if any results were obtained from the DNA extract, such as sequencing.</t>
+  </si>
+  <si>
+    <t>This table holds any microbes that need to be recorded. This information is useful if any results were obtained from the microbe itself, such as inhibition of fungal growth or increase in plant vigor.</t>
+  </si>
+  <si>
+    <t>This table holds any cultures that need to be recorded. This is useful if there are any measurements from the cultures, such as controlled vocabulary descriptions. Also, it is useful for if a separate observation units, such as DNA, was extracted from a culture. In that case it would be possible to store the culture info and match it to the DNA info.</t>
+  </si>
+  <si>
+    <t>This table holds all sample information. This is useful if measurements were obtained from specific seed samples, such as toxin level readings or respiration results or density results.</t>
+  </si>
+  <si>
+    <t>This table holds all tissues that need to be recorded. This is useful if results came from specific tissues. Also, this is useful if a different observation unit came from a tissue, for example if a microbe came from a tissue, it would be possible to record and track both.</t>
+  </si>
+  <si>
+    <t>This table holds any specific wells that need to be recorded. Sometimes it is necessary to track individual wells and it is useful for keeping trak of exactly what is in each well. Also, useful if results are associated to individual wells.</t>
+  </si>
+  <si>
+    <t>This table holds any plate info that needs to be recorded. This is useful for example, if individual wells in a 96-well plate are recorded, then those wells will have a corresponding plate in this table. This table can store a variety of plate info, not only 96-well.</t>
+  </si>
+  <si>
+    <t>lab_ObsTracker</t>
+  </si>
+  <si>
+    <t>The medium that the culture was grown in. Specifically this is the id from lab_medium. Media names are unique and so should be used to select this: medium_id = Medium(media_name).id</t>
+  </si>
+  <si>
+    <t>obs_culture_id</t>
+  </si>
+  <si>
+    <t>obs_dna_id</t>
+  </si>
+  <si>
+    <t>obs_microbe_id</t>
+  </si>
+  <si>
+    <t>obs_plant_id</t>
+  </si>
+  <si>
+    <t>obs_plate_id</t>
+  </si>
+  <si>
+    <t>obs_sample_id</t>
+  </si>
+  <si>
+    <t>obs_tissue_id</t>
+  </si>
+  <si>
+    <t>obs_well_id</t>
+  </si>
+  <si>
+    <t>obs_env_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This table links the above observation units (ObsPlant, ObsDNA, ObsEnv, ObsMicrobe, ObsCulture, ObsSample, ObsTissue, ObsWell, ObsRow, ObsPlate) to the measurement table, the experiment table, and to any dependent tables such as seed stocks, locations, fields, users, etc. The FKs to the obs units are one-to-one, meaning for every entry in an obs unit there is one entry in the obs tracker. Many queries can be directed to this table, for easy results. </t>
+  </si>
+  <si>
+    <t>A controlled vocab for the type of observation unit being tracked. Either: ObsPlant, ObsDNA, ObsEnv, ObsMicrobe, ObsCulture, ObsSample, ObsTissue, ObsWell, ObsRow, ObsPlate</t>
+  </si>
+  <si>
+    <t>If a user is associated to the observation unit. For example: a user created a culture. Specifically this is an id from auth_user. Usernames should be used to select this because they are unique.</t>
+  </si>
+  <si>
+    <t>If a location is associated to the observation unit. For example: the location of a plate or culture. Specifically this is the id from lab_location. Location names should be used to select this because they are unique.</t>
+  </si>
+  <si>
+    <t>The experiment that an observation unit belongs to. Specifically this is the id from lab_experiment. Experiment names should be used to select this.</t>
+  </si>
+  <si>
+    <t>If the observation unit is associated to a field. For example: a row is planted in a field. Specifically this is the id from lab_ObsRow. Row IDs should be used to select this because they are unique.</t>
+  </si>
+  <si>
+    <t>If the observation unit is associated to an isolate. For example: a DNA extract was from a specific isolate. Specifically this is the id from lab_isolate. Isolate IDs should be used to select this because they are unique.</t>
+  </si>
+  <si>
+    <t>If the observation unit is assocaited to a seed stock. For example: a row was planted with specific seed. Specifically this is the id from lab_stock. Seed IDs should be used to select this because they are unique.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the observation unit is associated to a collecting of seed or isolates. For example: seed was collected from a row or an isolate was collected from a tissue. Specifically this is the id from lab_collecting. </t>
+  </si>
+  <si>
+    <t>obs_entity_type</t>
+  </si>
+  <si>
+    <t>A one to one relationship to lab_ObsCulture. Specifically this is the id from lab_ObsCulture. If the obs_entity_type is ObsCulture, then a relevant culture will be recorded here. If the obs_entity_type is not ObsCulture, then obs_culture_id will be 1 and will point to a dummy "No Culture" result. Culture IDs should be used to select this because they are unique.</t>
+  </si>
+  <si>
+    <t>A one to one relationship to lab_ObsDNA. Specifically this is the id from lab_ObsDNA. If the obs_entity_type is ObsDNA, then a relevant record will be here. If the obs_entity_type is not ObsDNA, then obs_dna_id will be 1 and will point to a dummy "No DNA" entry. DNA IDs should be used to select this because they are unique.</t>
+  </si>
+  <si>
+    <t>A one to one relationship to lab_ObsMicrobe. Specifically this is the id from lab_ObsMicrobe. If the obs_entity_type is ObsMicrobe, then a relevant record will be here. If the obs_entity_type is not ObsMicrobe, then obs_microbe_id will be 1 and will point to a dummy "No Microbe" entry. Microbe IDs should be used to select this because they are unique.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A one to one relationship to lab_ObsPlant. Specifically this is the id from lab_ObsPlant. If the obs_entity_type is ObsPlant, then a relevant result will be here. If the obs_entity_type is not ObsPlant, then the obs_plant_id will be 1 and will point to a dummy "No Plant" entry. Plant IDs should be used to select this because they are unique. </t>
+  </si>
+  <si>
+    <t>A one to one relationship to lab_ObsPlate. Specfically this is the id from lab_ObsPlate. If the obs_entity_type is ObsPlate, then a relevant result will be here. If the obs_entity_type is not ObsPlate, then the obs_plate_id will be 1 and will point to a dummy "No Plate" entry. Plate IDs should be used to select this because they are unique.</t>
+  </si>
+  <si>
+    <t>A one to one relationship to lab_ObsRow. Specifically this is the id from lab_ObsRow. If the obs_entity_id is ObsRow, then a relevant result will be here. If the obs_entity_id is not ObsRow, then the obs_row_id will be 1 and will point to a dummy "No Row" entry. Row IDs should be used to select this because they are unique.</t>
+  </si>
+  <si>
+    <t>A one to one relationship to lab_ObsSample. Specifically this is the id from lab_ObsSample. If the obs_entity_id is ObsSample, then a relevant result will be here. If the obs_entity_id is not ObsSample, then the obs_sample_id will be 1 and will point to a dummy "No Sample" entry. Sample IDs should be used to select this because they are unique.</t>
+  </si>
+  <si>
+    <t>A one to one relationship to lab_ObsTissue. Specifically this is the id from lab_ObsTissue. If the obs_entity_id is ObsTissue, then a relevant result will be here. If the obs_entity_id is not ObsTissue, then the obs_tissue_id will be 1 and will point to a dummy "No Tissue" entry. Tissue IDs should be used to select this because they are unique.</t>
+  </si>
+  <si>
+    <t>A one to one relationship to lab_ObsWell. Specifically this is the id from lab_ObsWell. If the obs_entity_id is ObsWell, then a relevant result will be here. If the obs_entity_id is not ObsWell, then the obs_well_id will be 1 and will point to a dummy "No Well" entry. Well IDs should be used to select this because they are unique.</t>
+  </si>
+  <si>
+    <t>A one to one relationship to lab_ObsEnv. Specifically this is the id from lab_ObsEnv. If the obs_entity_id is ObsEnv, then a relevant result will be here. If the obs_entity_id is not ObsEnv, then the obs_env_id will be 1 and will point to a dummy "No Environment" entry. Environment IDs should be used to select this because they are unique.</t>
+  </si>
+  <si>
+    <t>lab_ObsTrackerSource</t>
+  </si>
+  <si>
+    <t>target_obs_id</t>
+  </si>
+  <si>
+    <t>source_obs_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The observation unit that is the product of other observation units. Those other observation units are the source_obs_id. </t>
+  </si>
+  <si>
+    <t>This table holds information about if an observation unit was from separate observation units. For example: If a tissue is from many plants, or if a well is from many tissues, or a culture is from many microbes, etc. For example: if a single well contains three different tissues, there would be three entries in this table with three identical target_obs_ids and three different source_obs_ids.</t>
+  </si>
+  <si>
+    <t>The observation unit that was the source of the target observation unit.</t>
   </si>
 </sst>
 </file>
@@ -1765,10 +1863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q271"/>
+  <dimension ref="A1:Q315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
-      <selection activeCell="C246" sqref="C246"/>
+    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="C187" sqref="C187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1786,7 +1884,7 @@
     </row>
     <row r="3" spans="1:17" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>247</v>
+        <v>187</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="6" t="s">
@@ -1826,7 +1924,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>340</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -1897,7 +1995,7 @@
     </row>
     <row r="13" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>246</v>
+        <v>186</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="6" t="s">
@@ -1923,7 +2021,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>340</v>
+        <v>279</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="30" x14ac:dyDescent="0.25">
@@ -1983,7 +2081,7 @@
     </row>
     <row r="22" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>245</v>
+        <v>185</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="6" t="s">
@@ -2009,7 +2107,7 @@
         <v>12</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>340</v>
+        <v>279</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2058,7 +2156,7 @@
     </row>
     <row r="30" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>244</v>
+        <v>184</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="6" t="s">
@@ -2084,7 +2182,7 @@
         <v>12</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>340</v>
+        <v>279</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2133,7 +2231,7 @@
     </row>
     <row r="38" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>243</v>
+        <v>183</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="6" t="s">
@@ -2159,7 +2257,7 @@
         <v>12</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>340</v>
+        <v>279</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -2274,7 +2372,7 @@
     </row>
     <row r="52" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>242</v>
+        <v>182</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="6" t="s">
@@ -2300,7 +2398,7 @@
         <v>12</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>340</v>
+        <v>279</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -2380,209 +2478,198 @@
         <v>82</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="61.5" x14ac:dyDescent="0.35">
-      <c r="A63" s="1" t="s">
+    <row r="64" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B63" s="1"/>
-      <c r="C63" s="6" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
+      <c r="B64" s="1"/>
+      <c r="C64" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B65" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C64" s="8" t="s">
+      <c r="C65" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>1</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>12</v>
       </c>
-      <c r="C65" s="7" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>20</v>
-      </c>
-      <c r="B66" t="s">
-        <v>13</v>
-      </c>
       <c r="C66" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A68" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B68" s="1"/>
-      <c r="C68" s="6" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C69" s="8" t="s">
-        <v>11</v>
+      <c r="B67" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>87</v>
+      </c>
+      <c r="B68" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>88</v>
+      </c>
+      <c r="B69" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>1</v>
+        <v>89</v>
       </c>
       <c r="B70" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>340</v>
+        <v>98</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B71" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="B72" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="B73" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B74" t="s">
         <v>14</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B75" t="s">
         <v>14</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>90</v>
+        <v>5</v>
       </c>
       <c r="B76" t="s">
         <v>14</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>91</v>
-      </c>
-      <c r="B77" t="s">
-        <v>14</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>92</v>
-      </c>
-      <c r="B78" t="s">
-        <v>14</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>93</v>
-      </c>
-      <c r="B79" t="s">
-        <v>14</v>
-      </c>
-      <c r="C79" s="7" t="s">
         <v>104</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B78" s="1"/>
+      <c r="C78" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>94</v>
+        <v>1</v>
       </c>
       <c r="B80" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>105</v>
+        <v>279</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="B81" t="s">
         <v>14</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="B82" t="s">
         <v>14</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -2593,16 +2680,16 @@
         <v>14</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B85" s="1"/>
       <c r="C85" s="6" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2624,267 +2711,254 @@
         <v>12</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>340</v>
+        <v>279</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>87</v>
+        <v>115</v>
       </c>
       <c r="B88" t="s">
         <v>13</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B89" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B90" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>114</v>
+        <v>5</v>
       </c>
       <c r="B91" t="s">
         <v>14</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>113</v>
-      </c>
-      <c r="B92" t="s">
-        <v>14</v>
-      </c>
-      <c r="C92" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>5</v>
-      </c>
-      <c r="B93" t="s">
-        <v>14</v>
-      </c>
-      <c r="C93" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
-      <c r="A95" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B95" s="1"/>
-      <c r="C95" s="6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A96" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B93" s="1"/>
+      <c r="C93" s="6" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B94" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C96" s="8" t="s">
+      <c r="C94" s="8" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>1</v>
+      </c>
+      <c r="B95" t="s">
+        <v>12</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>125</v>
+      </c>
+      <c r="B96" t="s">
+        <v>14</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>1</v>
+        <v>341</v>
       </c>
       <c r="B97" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>340</v>
+        <v>142</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>87</v>
+        <v>23</v>
       </c>
       <c r="B98" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>97</v>
+        <v>143</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>7</v>
+        <v>342</v>
       </c>
       <c r="B99" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>122</v>
+        <v>343</v>
       </c>
       <c r="B100" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>123</v>
+        <v>5</v>
       </c>
       <c r="B101" t="s">
         <v>14</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>124</v>
-      </c>
-      <c r="B102" t="s">
-        <v>14</v>
-      </c>
-      <c r="C102" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>5</v>
-      </c>
-      <c r="B103" t="s">
-        <v>14</v>
-      </c>
-      <c r="C103" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" ht="61.5" x14ac:dyDescent="0.35">
-      <c r="A105" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B105" s="1"/>
-      <c r="C105" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A106" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="A103" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B103" s="1"/>
+      <c r="C103" s="6" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A104" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="B104" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C106" s="8" t="s">
+      <c r="C104" s="8" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>1</v>
+      </c>
+      <c r="B105" t="s">
+        <v>12</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>139</v>
+      </c>
+      <c r="B106" t="s">
+        <v>14</v>
+      </c>
+      <c r="C106" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>1</v>
+        <v>140</v>
       </c>
       <c r="B107" t="s">
-        <v>12</v>
-      </c>
-      <c r="C107" s="7" t="s">
-        <v>340</v>
+        <v>14</v>
+      </c>
+      <c r="C107" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>87</v>
+        <v>5</v>
       </c>
       <c r="B108" t="s">
-        <v>13</v>
-      </c>
-      <c r="C108" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>6</v>
-      </c>
-      <c r="B109" t="s">
-        <v>13</v>
-      </c>
-      <c r="C109" s="7" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>133</v>
-      </c>
-      <c r="B110" t="s">
-        <v>13</v>
-      </c>
-      <c r="C110" s="7" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>134</v>
-      </c>
-      <c r="B111" t="s">
-        <v>13</v>
-      </c>
-      <c r="C111" s="7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="C108" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="A110" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B110" s="1"/>
+      <c r="C110" s="6" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A111" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C111" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>135</v>
+        <v>1</v>
       </c>
       <c r="B112" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>190</v>
+        <v>279</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="B113" t="s">
         <v>13</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>189</v>
+        <v>364</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -2892,730 +2966,694 @@
         <v>137</v>
       </c>
       <c r="B114" t="s">
-        <v>13</v>
-      </c>
-      <c r="C114" s="7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>138</v>
       </c>
       <c r="B115" t="s">
-        <v>13</v>
-      </c>
-      <c r="C115" s="7" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="C115" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B116" t="s">
-        <v>13</v>
-      </c>
-      <c r="C116" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="C116" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>140</v>
+        <v>346</v>
       </c>
       <c r="B117" t="s">
-        <v>13</v>
-      </c>
-      <c r="C117" s="7" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="C117" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>141</v>
+        <v>347</v>
       </c>
       <c r="B118" t="s">
-        <v>13</v>
-      </c>
-      <c r="C118" s="7" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="C118" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>142</v>
+        <v>348</v>
       </c>
       <c r="B119" t="s">
-        <v>13</v>
-      </c>
-      <c r="C119" s="7" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="C119" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>143</v>
+        <v>5</v>
       </c>
       <c r="B120" t="s">
-        <v>13</v>
-      </c>
-      <c r="C120" s="7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>144</v>
-      </c>
-      <c r="B121" t="s">
-        <v>13</v>
-      </c>
-      <c r="C121" s="7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>145</v>
-      </c>
-      <c r="B122" t="s">
-        <v>13</v>
-      </c>
-      <c r="C122" s="7" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>146</v>
-      </c>
-      <c r="B123" t="s">
-        <v>14</v>
-      </c>
-      <c r="C123" s="7" t="s">
-        <v>200</v>
+        <v>14</v>
+      </c>
+      <c r="C120" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A122" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B122" s="1"/>
+      <c r="C122" s="6" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A123" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C123" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>147</v>
+        <v>1</v>
       </c>
       <c r="B124" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C124" s="7" t="s">
-        <v>201</v>
+        <v>279</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B125" t="s">
         <v>14</v>
       </c>
-      <c r="C125" s="7" t="s">
-        <v>202</v>
+      <c r="C125" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="B126" t="s">
         <v>14</v>
       </c>
-      <c r="C126" s="7" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C126" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>150</v>
+        <v>236</v>
       </c>
       <c r="B127" t="s">
         <v>14</v>
       </c>
-      <c r="C127" s="7" t="s">
-        <v>204</v>
+      <c r="C127" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>151</v>
+        <v>92</v>
       </c>
       <c r="B128" t="s">
         <v>14</v>
       </c>
-      <c r="C128" s="7" t="s">
-        <v>205</v>
+      <c r="C128" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>152</v>
+        <v>5</v>
       </c>
       <c r="B129" t="s">
         <v>14</v>
       </c>
-      <c r="C129" s="7" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>153</v>
-      </c>
-      <c r="B130" t="s">
-        <v>14</v>
-      </c>
-      <c r="C130" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>154</v>
-      </c>
-      <c r="B131" t="s">
-        <v>14</v>
-      </c>
-      <c r="C131" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>155</v>
-      </c>
-      <c r="B132" t="s">
-        <v>14</v>
-      </c>
-      <c r="C132" t="s">
-        <v>209</v>
+      <c r="C129" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="A131" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B131" s="1"/>
+      <c r="C131" s="6" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A132" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C132" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>156</v>
+        <v>1</v>
       </c>
       <c r="B133" t="s">
-        <v>14</v>
-      </c>
-      <c r="C133" t="s">
-        <v>210</v>
+        <v>12</v>
+      </c>
+      <c r="C133" s="7" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>157</v>
+        <v>126</v>
       </c>
       <c r="B134" t="s">
         <v>14</v>
       </c>
       <c r="C134" t="s">
-        <v>211</v>
+        <v>147</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="B135" t="s">
         <v>14</v>
       </c>
       <c r="C135" t="s">
-        <v>224</v>
+        <v>148</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>159</v>
+        <v>128</v>
       </c>
       <c r="B136" t="s">
         <v>14</v>
       </c>
       <c r="C136" t="s">
-        <v>225</v>
+        <v>149</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>160</v>
+        <v>351</v>
       </c>
       <c r="B137" t="s">
         <v>14</v>
       </c>
       <c r="C137" t="s">
-        <v>226</v>
+        <v>150</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>161</v>
+        <v>5</v>
       </c>
       <c r="B138" t="s">
         <v>14</v>
       </c>
       <c r="C138" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>162</v>
-      </c>
-      <c r="B139" t="s">
-        <v>14</v>
-      </c>
-      <c r="C139" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>163</v>
-      </c>
-      <c r="B140" t="s">
-        <v>14</v>
-      </c>
-      <c r="C140" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>164</v>
-      </c>
-      <c r="B141" t="s">
-        <v>14</v>
-      </c>
-      <c r="C141" t="s">
-        <v>230</v>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="A140" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B140" s="1"/>
+      <c r="C140" s="6" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A141" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B141" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C141" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>165</v>
+        <v>1</v>
       </c>
       <c r="B142" t="s">
-        <v>14</v>
-      </c>
-      <c r="C142" t="s">
-        <v>231</v>
+        <v>12</v>
+      </c>
+      <c r="C142" s="7" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>166</v>
+        <v>135</v>
       </c>
       <c r="B143" t="s">
         <v>14</v>
       </c>
       <c r="C143" t="s">
-        <v>232</v>
+        <v>159</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="B144" t="s">
         <v>14</v>
       </c>
       <c r="C144" t="s">
-        <v>233</v>
+        <v>160</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="B145" t="s">
         <v>14</v>
       </c>
       <c r="C145" t="s">
-        <v>234</v>
+        <v>161</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>169</v>
+        <v>353</v>
       </c>
       <c r="B146" t="s">
         <v>14</v>
       </c>
       <c r="C146" t="s">
-        <v>235</v>
+        <v>162</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>170</v>
+        <v>5</v>
       </c>
       <c r="B147" t="s">
         <v>14</v>
       </c>
       <c r="C147" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>171</v>
-      </c>
-      <c r="B148" t="s">
-        <v>14</v>
-      </c>
-      <c r="C148" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>173</v>
-      </c>
-      <c r="B149" t="s">
-        <v>14</v>
-      </c>
-      <c r="C149" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>172</v>
-      </c>
-      <c r="B150" t="s">
-        <v>14</v>
-      </c>
-      <c r="C150" t="s">
-        <v>221</v>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="A149" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B149" s="1"/>
+      <c r="C149" s="6" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A150" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B150" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C150" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>174</v>
+        <v>1</v>
       </c>
       <c r="B151" t="s">
-        <v>14</v>
-      </c>
-      <c r="C151" t="s">
-        <v>222</v>
+        <v>12</v>
+      </c>
+      <c r="C151" s="7" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>175</v>
+        <v>129</v>
       </c>
       <c r="B152" t="s">
         <v>14</v>
       </c>
       <c r="C152" t="s">
-        <v>223</v>
+        <v>164</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>176</v>
+        <v>130</v>
       </c>
       <c r="B153" t="s">
         <v>14</v>
       </c>
-      <c r="C153" s="3" t="s">
-        <v>212</v>
+      <c r="C153" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>177</v>
+        <v>23</v>
       </c>
       <c r="B154" t="s">
         <v>14</v>
       </c>
       <c r="C154" t="s">
-        <v>213</v>
+        <v>166</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>178</v>
+        <v>355</v>
       </c>
       <c r="B155" t="s">
         <v>14</v>
       </c>
       <c r="C155" t="s">
-        <v>214</v>
+        <v>167</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>179</v>
+        <v>91</v>
       </c>
       <c r="B156" t="s">
         <v>14</v>
       </c>
       <c r="C156" t="s">
-        <v>215</v>
+        <v>168</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>180</v>
+        <v>131</v>
       </c>
       <c r="B157" t="s">
         <v>14</v>
       </c>
       <c r="C157" t="s">
-        <v>216</v>
+        <v>169</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>181</v>
+        <v>132</v>
       </c>
       <c r="B158" t="s">
         <v>14</v>
       </c>
       <c r="C158" t="s">
-        <v>217</v>
+        <v>170</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>182</v>
+        <v>5</v>
       </c>
       <c r="B159" t="s">
         <v>14</v>
       </c>
       <c r="C159" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>183</v>
-      </c>
-      <c r="B160" t="s">
-        <v>14</v>
-      </c>
-      <c r="C160" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>184</v>
-      </c>
-      <c r="B161" t="s">
-        <v>14</v>
-      </c>
-      <c r="C161" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>185</v>
-      </c>
-      <c r="B162" t="s">
-        <v>14</v>
-      </c>
-      <c r="C162" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A164" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="B164" s="1"/>
-      <c r="C164" s="6" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A165" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A161" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B161" s="1"/>
+      <c r="C161" s="6" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A162" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B165" s="4" t="s">
+      <c r="B162" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C165" s="8" t="s">
+      <c r="C162" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="166" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A166" s="5" t="s">
-        <v>253</v>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>1</v>
+      </c>
+      <c r="B163" t="s">
+        <v>12</v>
+      </c>
+      <c r="C163" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>383</v>
+      </c>
+      <c r="B164" t="s">
+        <v>14</v>
+      </c>
+      <c r="C164" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>6</v>
+      </c>
+      <c r="B165" t="s">
+        <v>13</v>
+      </c>
+      <c r="C165" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>124</v>
       </c>
       <c r="B166" t="s">
-        <v>12</v>
-      </c>
-      <c r="C166" s="7" t="s">
-        <v>340</v>
+        <v>13</v>
+      </c>
+      <c r="C166" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>248</v>
+        <v>20</v>
       </c>
       <c r="B167" t="s">
-        <v>14</v>
-      </c>
-      <c r="C167" s="7" t="s">
-        <v>258</v>
+        <v>13</v>
+      </c>
+      <c r="C167" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>249</v>
+        <v>7</v>
       </c>
       <c r="B168" t="s">
-        <v>14</v>
-      </c>
-      <c r="C168" s="7" t="s">
-        <v>259</v>
+        <v>13</v>
+      </c>
+      <c r="C168" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B169" t="s">
-        <v>14</v>
-      </c>
-      <c r="C169" s="7" t="s">
-        <v>262</v>
+        <v>13</v>
+      </c>
+      <c r="C169" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>251</v>
+        <v>108</v>
       </c>
       <c r="B170" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C170" t="s">
-        <v>261</v>
+        <v>381</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>252</v>
+        <v>220</v>
       </c>
       <c r="B171" t="s">
-        <v>14</v>
-      </c>
-      <c r="C171" s="7" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
-      <c r="A173" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="B173" s="1"/>
-      <c r="C173" s="6" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A174" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B174" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C174" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="C171" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>365</v>
+      </c>
+      <c r="B172" t="s">
+        <v>13</v>
+      </c>
+      <c r="C172" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>366</v>
+      </c>
+      <c r="B173" t="s">
+        <v>13</v>
+      </c>
+      <c r="C173" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>367</v>
+      </c>
+      <c r="B174" t="s">
+        <v>13</v>
+      </c>
+      <c r="C174" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>1</v>
+        <v>368</v>
       </c>
       <c r="B175" t="s">
-        <v>12</v>
-      </c>
-      <c r="C175" s="7" t="s">
-        <v>340</v>
+        <v>13</v>
+      </c>
+      <c r="C175" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>87</v>
+        <v>369</v>
       </c>
       <c r="B176" t="s">
         <v>13</v>
       </c>
-      <c r="C176" s="7" t="s">
-        <v>97</v>
+      <c r="C176" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>254</v>
+        <v>107</v>
       </c>
       <c r="B177" t="s">
         <v>13</v>
       </c>
       <c r="C177" t="s">
-        <v>267</v>
+        <v>389</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>6</v>
+        <v>370</v>
       </c>
       <c r="B178" t="s">
         <v>13</v>
       </c>
       <c r="C178" t="s">
-        <v>268</v>
+        <v>390</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>255</v>
+        <v>371</v>
       </c>
       <c r="B179" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C179" t="s">
-        <v>264</v>
+        <v>391</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>256</v>
+        <v>372</v>
       </c>
       <c r="B180" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C180" t="s">
-        <v>265</v>
+        <v>392</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>5</v>
+        <v>373</v>
       </c>
       <c r="B181" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C181" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C182"/>
+    </row>
+    <row r="183" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A183" s="1" t="s">
-        <v>269</v>
+        <v>394</v>
       </c>
       <c r="B183" s="1"/>
       <c r="C183" s="6" t="s">
-        <v>270</v>
+        <v>398</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -3629,860 +3667,1279 @@
         <v>11</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>1</v>
+    <row r="185" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A185" s="5" t="s">
+        <v>193</v>
       </c>
       <c r="B185" t="s">
         <v>12</v>
       </c>
       <c r="C185" s="7" t="s">
-        <v>340</v>
+        <v>279</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>278</v>
+        <v>395</v>
       </c>
       <c r="B186" t="s">
         <v>13</v>
       </c>
       <c r="C186" s="7" t="s">
-        <v>312</v>
+        <v>397</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>271</v>
+        <v>396</v>
       </c>
       <c r="B187" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C187" s="7" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>272</v>
-      </c>
-      <c r="B188" t="s">
-        <v>14</v>
-      </c>
-      <c r="C188" s="7" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>273</v>
-      </c>
-      <c r="B189" t="s">
-        <v>14</v>
-      </c>
-      <c r="C189" s="7" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>274</v>
-      </c>
-      <c r="B190" t="s">
-        <v>14</v>
-      </c>
-      <c r="C190" s="7" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>275</v>
+        <v>399</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A189" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B189" s="1"/>
+      <c r="C189" s="6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A190" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B190" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C190" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A191" s="5" t="s">
+        <v>193</v>
       </c>
       <c r="B191" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C191" s="7" t="s">
-        <v>317</v>
+        <v>279</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>276</v>
+        <v>188</v>
       </c>
       <c r="B192" t="s">
         <v>14</v>
       </c>
       <c r="C192" s="7" t="s">
-        <v>318</v>
+        <v>198</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>277</v>
+        <v>189</v>
       </c>
       <c r="B193" t="s">
         <v>14</v>
       </c>
       <c r="C193" s="7" t="s">
-        <v>319</v>
+        <v>199</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>5</v>
+        <v>190</v>
       </c>
       <c r="B194" t="s">
         <v>14</v>
       </c>
       <c r="C194" s="7" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A196" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="B196" s="1"/>
-      <c r="C196" s="6" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A197" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>191</v>
+      </c>
+      <c r="B195" t="s">
+        <v>14</v>
+      </c>
+      <c r="C195" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>192</v>
+      </c>
+      <c r="B196" t="s">
+        <v>14</v>
+      </c>
+      <c r="C196" s="7" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="A198" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B198" s="1"/>
+      <c r="C198" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A199" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B197" s="4" t="s">
+      <c r="B199" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C197" s="8" t="s">
+      <c r="C199" s="8" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
-        <v>1</v>
-      </c>
-      <c r="B198" t="s">
-        <v>12</v>
-      </c>
-      <c r="C198" s="7" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
-        <v>280</v>
-      </c>
-      <c r="B199" t="s">
-        <v>13</v>
-      </c>
-      <c r="C199" s="7" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>281</v>
+        <v>1</v>
       </c>
       <c r="B200" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C200" s="7" t="s">
-        <v>321</v>
+        <v>279</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>282</v>
+        <v>338</v>
       </c>
       <c r="B201" t="s">
         <v>13</v>
       </c>
       <c r="C201" s="7" t="s">
-        <v>322</v>
+        <v>339</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C202"/>
-    </row>
-    <row r="203" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
-      <c r="A203" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="B203" s="1"/>
-      <c r="C203" s="6" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A204" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B204" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C204" s="8" t="s">
-        <v>11</v>
+      <c r="A202" t="s">
+        <v>194</v>
+      </c>
+      <c r="B202" t="s">
+        <v>13</v>
+      </c>
+      <c r="C202" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>6</v>
+      </c>
+      <c r="B203" t="s">
+        <v>13</v>
+      </c>
+      <c r="C203" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>195</v>
+      </c>
+      <c r="B204" t="s">
+        <v>14</v>
+      </c>
+      <c r="C204" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>1</v>
+        <v>196</v>
       </c>
       <c r="B205" t="s">
-        <v>12</v>
-      </c>
-      <c r="C205" s="7" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="C205" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>87</v>
+        <v>5</v>
       </c>
       <c r="B206" t="s">
-        <v>13</v>
-      </c>
-      <c r="C206" s="7" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
-        <v>7</v>
-      </c>
-      <c r="B207" t="s">
-        <v>13</v>
-      </c>
-      <c r="C207" s="7" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
-        <v>6</v>
-      </c>
-      <c r="B208" t="s">
-        <v>13</v>
-      </c>
-      <c r="C208" s="7" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
-        <v>284</v>
-      </c>
-      <c r="B209" t="s">
-        <v>14</v>
-      </c>
-      <c r="C209" s="7" t="s">
-        <v>329</v>
+        <v>14</v>
+      </c>
+      <c r="C206" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A208" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B208" s="1"/>
+      <c r="C208" s="6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A209" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B209" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C209" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>285</v>
+        <v>1</v>
       </c>
       <c r="B210" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C210" s="7" t="s">
-        <v>330</v>
+        <v>279</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>5</v>
+        <v>218</v>
       </c>
       <c r="B211" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C211" s="7" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
-      <c r="A213" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="B213" s="1"/>
-      <c r="C213" s="6" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A214" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B214" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C214" s="8" t="s">
-        <v>11</v>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>211</v>
+      </c>
+      <c r="B212" t="s">
+        <v>14</v>
+      </c>
+      <c r="C212" s="7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>212</v>
+      </c>
+      <c r="B213" t="s">
+        <v>14</v>
+      </c>
+      <c r="C213" s="7" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>213</v>
+      </c>
+      <c r="B214" t="s">
+        <v>14</v>
+      </c>
+      <c r="C214" s="7" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>1</v>
+        <v>214</v>
       </c>
       <c r="B215" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C215" s="7" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>53</v>
+        <v>215</v>
       </c>
       <c r="B216" t="s">
         <v>14</v>
       </c>
       <c r="C216" s="7" t="s">
-        <v>333</v>
+        <v>257</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>54</v>
+        <v>216</v>
       </c>
       <c r="B217" t="s">
         <v>14</v>
       </c>
       <c r="C217" s="7" t="s">
-        <v>334</v>
+        <v>258</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>73</v>
+        <v>217</v>
       </c>
       <c r="B218" t="s">
         <v>14</v>
       </c>
       <c r="C218" s="7" t="s">
-        <v>335</v>
+        <v>259</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>71</v>
+        <v>5</v>
       </c>
       <c r="B219" t="s">
         <v>14</v>
       </c>
       <c r="C219" s="7" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
-        <v>55</v>
-      </c>
-      <c r="B220" t="s">
-        <v>14</v>
-      </c>
-      <c r="C220" s="7" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
-        <v>5</v>
-      </c>
-      <c r="B221" t="s">
-        <v>14</v>
-      </c>
-      <c r="C221" s="7" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A223" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="B223" s="1"/>
-      <c r="C223" s="6" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A224" s="4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A221" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B221" s="1"/>
+      <c r="C221" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A222" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B224" s="4" t="s">
+      <c r="B222" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C224" s="8" t="s">
+      <c r="C222" s="8" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>1</v>
+      </c>
+      <c r="B223" t="s">
+        <v>12</v>
+      </c>
+      <c r="C223" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>220</v>
+      </c>
+      <c r="B224" t="s">
+        <v>13</v>
+      </c>
+      <c r="C224" s="7" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>1</v>
+        <v>221</v>
       </c>
       <c r="B225" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C225" s="7" t="s">
-        <v>340</v>
+        <v>261</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>288</v>
+        <v>222</v>
       </c>
       <c r="B226" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C226" s="7" t="s">
-        <v>346</v>
+        <v>262</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A227" t="s">
-        <v>289</v>
-      </c>
-      <c r="B227" t="s">
-        <v>14</v>
-      </c>
-      <c r="C227" s="7" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A228" t="s">
-        <v>290</v>
-      </c>
-      <c r="B228" t="s">
-        <v>14</v>
-      </c>
-      <c r="C228" s="7" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A229" t="s">
-        <v>291</v>
-      </c>
-      <c r="B229" t="s">
-        <v>14</v>
-      </c>
-      <c r="C229" s="7" t="s">
-        <v>342</v>
+      <c r="C227"/>
+    </row>
+    <row r="228" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="A228" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B228" s="1"/>
+      <c r="C228" s="6" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A229" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B229" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C229" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>292</v>
+        <v>1</v>
       </c>
       <c r="B230" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C230" s="7" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>293</v>
+        <v>85</v>
       </c>
       <c r="B231" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C231" s="7" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>294</v>
+        <v>7</v>
       </c>
       <c r="B232" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C232" s="7" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
-      <c r="A234" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="B234" s="1"/>
-      <c r="C234" s="6" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A235" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B235" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C235" s="8" t="s">
-        <v>11</v>
+        <v>267</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>6</v>
+      </c>
+      <c r="B233" t="s">
+        <v>13</v>
+      </c>
+      <c r="C233" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>224</v>
+      </c>
+      <c r="B234" t="s">
+        <v>14</v>
+      </c>
+      <c r="C234" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>225</v>
+      </c>
+      <c r="B235" t="s">
+        <v>14</v>
+      </c>
+      <c r="C235" s="7" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B236" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C236" s="7" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A237" t="s">
-        <v>112</v>
-      </c>
-      <c r="B237" t="s">
-        <v>13</v>
-      </c>
-      <c r="C237" s="7" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A238" t="s">
-        <v>134</v>
-      </c>
-      <c r="B238" t="s">
-        <v>13</v>
-      </c>
-      <c r="C238" s="7" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A239" t="s">
-        <v>296</v>
-      </c>
-      <c r="B239" t="s">
-        <v>14</v>
-      </c>
-      <c r="C239" s="7" t="s">
-        <v>352</v>
+        <v>271</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="A238" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B238" s="1"/>
+      <c r="C238" s="6" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A239" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B239" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C239" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>297</v>
+        <v>1</v>
       </c>
       <c r="B240" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C240" s="7" t="s">
-        <v>353</v>
+        <v>279</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="B241" t="s">
         <v>14</v>
       </c>
       <c r="C241" s="7" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A243" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="B243" s="1"/>
-      <c r="C243" s="6" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A244" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B244" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C244" s="8" t="s">
-        <v>11</v>
+        <v>273</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>54</v>
+      </c>
+      <c r="B242" t="s">
+        <v>14</v>
+      </c>
+      <c r="C242" s="7" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>73</v>
+      </c>
+      <c r="B243" t="s">
+        <v>14</v>
+      </c>
+      <c r="C243" s="7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>71</v>
+      </c>
+      <c r="B244" t="s">
+        <v>14</v>
+      </c>
+      <c r="C244" s="7" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B245" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C245" s="7" t="s">
-        <v>340</v>
+        <v>277</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="B246" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C246" s="7" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A247" t="s">
-        <v>300</v>
-      </c>
-      <c r="B247" t="s">
-        <v>14</v>
-      </c>
-      <c r="C247" s="3" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A248" t="s">
-        <v>299</v>
-      </c>
-      <c r="B248" t="s">
-        <v>14</v>
-      </c>
-      <c r="C248" s="3" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A249" t="s">
-        <v>301</v>
-      </c>
-      <c r="B249" t="s">
-        <v>14</v>
-      </c>
-      <c r="C249" s="3" t="s">
-        <v>358</v>
+        <v>278</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A248" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B248" s="1"/>
+      <c r="C248" s="6" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A249" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B249" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C249" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>302</v>
+        <v>1</v>
       </c>
       <c r="B250" t="s">
-        <v>14</v>
-      </c>
-      <c r="C250" s="3" t="s">
-        <v>359</v>
+        <v>12</v>
+      </c>
+      <c r="C250" s="7" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>303</v>
+        <v>228</v>
       </c>
       <c r="B251" t="s">
         <v>14</v>
       </c>
-      <c r="C251" s="3" t="s">
-        <v>360</v>
+      <c r="C251" s="7" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>304</v>
+        <v>229</v>
       </c>
       <c r="B252" t="s">
         <v>14</v>
       </c>
-      <c r="C252" s="3" t="s">
-        <v>361</v>
+      <c r="C252" s="7" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>5</v>
+        <v>230</v>
       </c>
       <c r="B253" t="s">
         <v>14</v>
       </c>
-      <c r="C253" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="255" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A255" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="B255" s="1"/>
-      <c r="C255" s="6" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="256" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A256" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B256" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C256" s="8" t="s">
-        <v>11</v>
+      <c r="C253" s="7" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>231</v>
+      </c>
+      <c r="B254" t="s">
+        <v>14</v>
+      </c>
+      <c r="C254" s="7" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>232</v>
+      </c>
+      <c r="B255" t="s">
+        <v>14</v>
+      </c>
+      <c r="C255" s="7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>233</v>
+      </c>
+      <c r="B256" t="s">
+        <v>14</v>
+      </c>
+      <c r="C256" s="7" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>1</v>
+        <v>234</v>
       </c>
       <c r="B257" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C257" s="7" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A258" t="s">
-        <v>278</v>
-      </c>
-      <c r="B258" t="s">
-        <v>13</v>
-      </c>
-      <c r="C258" s="7" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="259" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A259" t="s">
-        <v>134</v>
-      </c>
-      <c r="B259" t="s">
-        <v>13</v>
-      </c>
-      <c r="C259" s="7" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A260" t="s">
-        <v>306</v>
-      </c>
-      <c r="B260" t="s">
-        <v>13</v>
-      </c>
-      <c r="C260" s="7" t="s">
-        <v>366</v>
+        <v>284</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="A259" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B259" s="1"/>
+      <c r="C259" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A260" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B260" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C260" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>307</v>
+        <v>1</v>
       </c>
       <c r="B261" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C261" s="7" t="s">
-        <v>367</v>
+        <v>279</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>308</v>
+        <v>108</v>
       </c>
       <c r="B262" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C262" s="7" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>309</v>
+        <v>124</v>
       </c>
       <c r="B263" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C263" s="7" t="s">
-        <v>369</v>
+        <v>290</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
+        <v>236</v>
+      </c>
+      <c r="B264" t="s">
+        <v>14</v>
+      </c>
+      <c r="C264" s="7" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>237</v>
+      </c>
+      <c r="B265" t="s">
+        <v>14</v>
+      </c>
+      <c r="C265" s="7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
         <v>5</v>
       </c>
-      <c r="B264" t="s">
-        <v>14</v>
-      </c>
-      <c r="C264" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="266" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A266" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="B266" s="1"/>
-      <c r="C266" s="6" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="267" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A267" s="4" t="s">
+      <c r="B266" t="s">
+        <v>14</v>
+      </c>
+      <c r="C266" s="7" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A268" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B268" s="1"/>
+      <c r="C268" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A269" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B267" s="4" t="s">
+      <c r="B269" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C267" s="8" t="s">
+      <c r="C269" s="8" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A268" t="s">
-        <v>1</v>
-      </c>
-      <c r="B268" t="s">
-        <v>12</v>
-      </c>
-      <c r="C268" s="7" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A269" t="s">
-        <v>291</v>
-      </c>
-      <c r="B269" t="s">
-        <v>14</v>
-      </c>
-      <c r="C269" s="7" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>311</v>
+        <v>1</v>
       </c>
       <c r="B270" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C270" s="7" t="s">
-        <v>373</v>
+        <v>279</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
+        <v>34</v>
+      </c>
+      <c r="B271" t="s">
+        <v>13</v>
+      </c>
+      <c r="C271" s="7" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>240</v>
+      </c>
+      <c r="B272" t="s">
+        <v>14</v>
+      </c>
+      <c r="C272" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>239</v>
+      </c>
+      <c r="B273" t="s">
+        <v>14</v>
+      </c>
+      <c r="C273" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>241</v>
+      </c>
+      <c r="B274" t="s">
+        <v>14</v>
+      </c>
+      <c r="C274" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>242</v>
+      </c>
+      <c r="B275" t="s">
+        <v>14</v>
+      </c>
+      <c r="C275" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>243</v>
+      </c>
+      <c r="B276" t="s">
+        <v>14</v>
+      </c>
+      <c r="C276" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>244</v>
+      </c>
+      <c r="B277" t="s">
+        <v>14</v>
+      </c>
+      <c r="C277" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
         <v>5</v>
       </c>
-      <c r="B271" t="s">
-        <v>14</v>
-      </c>
-      <c r="C271" s="7" t="s">
-        <v>374</v>
+      <c r="B278" t="s">
+        <v>14</v>
+      </c>
+      <c r="C278" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A280" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B280" s="1"/>
+      <c r="C280" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A281" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B281" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C281" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>1</v>
+      </c>
+      <c r="B282" t="s">
+        <v>12</v>
+      </c>
+      <c r="C282" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>218</v>
+      </c>
+      <c r="B283" t="s">
+        <v>13</v>
+      </c>
+      <c r="C283" s="7" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>124</v>
+      </c>
+      <c r="B284" t="s">
+        <v>13</v>
+      </c>
+      <c r="C284" s="7" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>246</v>
+      </c>
+      <c r="B285" t="s">
+        <v>13</v>
+      </c>
+      <c r="C285" s="7" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>247</v>
+      </c>
+      <c r="B286" t="s">
+        <v>14</v>
+      </c>
+      <c r="C286" s="7" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>248</v>
+      </c>
+      <c r="B287" t="s">
+        <v>14</v>
+      </c>
+      <c r="C287" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>249</v>
+      </c>
+      <c r="B288" t="s">
+        <v>14</v>
+      </c>
+      <c r="C288" s="7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>5</v>
+      </c>
+      <c r="B289" t="s">
+        <v>14</v>
+      </c>
+      <c r="C289" s="7" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A291" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B291" s="1"/>
+      <c r="C291" s="6" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A292" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B292" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C292" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>1</v>
+      </c>
+      <c r="B293" t="s">
+        <v>12</v>
+      </c>
+      <c r="C293" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>231</v>
+      </c>
+      <c r="B294" t="s">
+        <v>14</v>
+      </c>
+      <c r="C294" s="7" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>251</v>
+      </c>
+      <c r="B295" t="s">
+        <v>14</v>
+      </c>
+      <c r="C295" s="7" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>5</v>
+      </c>
+      <c r="B296" t="s">
+        <v>14</v>
+      </c>
+      <c r="C296" s="7" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A298" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B298" s="1"/>
+      <c r="C298" s="6" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A299" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B299" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C299" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>1</v>
+      </c>
+      <c r="B300" t="s">
+        <v>12</v>
+      </c>
+      <c r="C300" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>322</v>
+      </c>
+      <c r="B301" t="s">
+        <v>14</v>
+      </c>
+      <c r="C301" s="7" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>317</v>
+      </c>
+      <c r="B302" t="s">
+        <v>14</v>
+      </c>
+      <c r="C302" s="7" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>318</v>
+      </c>
+      <c r="B303" t="s">
+        <v>14</v>
+      </c>
+      <c r="C303" s="7" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>319</v>
+      </c>
+      <c r="B304" t="s">
+        <v>14</v>
+      </c>
+      <c r="C304" s="7" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>5</v>
+      </c>
+      <c r="B305" t="s">
+        <v>14</v>
+      </c>
+      <c r="C305" s="7" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A307" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B307" s="1"/>
+      <c r="C307" s="6" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A308" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B308" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C308" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>1</v>
+      </c>
+      <c r="B309" t="s">
+        <v>12</v>
+      </c>
+      <c r="C309" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>317</v>
+      </c>
+      <c r="B310" t="s">
+        <v>13</v>
+      </c>
+      <c r="C310" s="7" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>328</v>
+      </c>
+      <c r="B311" t="s">
+        <v>14</v>
+      </c>
+      <c r="C311" s="7" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>329</v>
+      </c>
+      <c r="B312" t="s">
+        <v>14</v>
+      </c>
+      <c r="C312" s="7" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>330</v>
+      </c>
+      <c r="B313" t="s">
+        <v>14</v>
+      </c>
+      <c r="C313" s="7" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>331</v>
+      </c>
+      <c r="B314" t="s">
+        <v>14</v>
+      </c>
+      <c r="C314" s="7" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>5</v>
+      </c>
+      <c r="B315" t="s">
+        <v>14</v>
+      </c>
+      <c r="C315" s="7" t="s">
+        <v>337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated db table dictionary
</commit_message>
<xml_diff>
--- a/NelsonLab Online Database Dictionary.xlsx
+++ b/NelsonLab Online Database Dictionary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="445">
   <si>
     <t>NelsonLab Online Database Dictionary</t>
   </si>
@@ -1411,9 +1411,6 @@
     <t xml:space="preserve">This table links the above observation units (ObsPlant, ObsDNA, ObsEnv, ObsMicrobe, ObsCulture, ObsSample, ObsTissue, ObsWell, ObsRow, ObsPlate) to the measurement table, the experiment table, and to any dependent tables such as seed stocks, locations, fields, users, etc. The FKs to the obs units are one-to-one, meaning for every entry in an obs unit there is one entry in the obs tracker. Many queries can be directed to this table, for easy results. </t>
   </si>
   <si>
-    <t>A controlled vocab for the type of observation unit being tracked. Either: ObsPlant, ObsDNA, ObsEnv, ObsMicrobe, ObsCulture, ObsSample, ObsTissue, ObsWell, ObsRow, ObsPlate</t>
-  </si>
-  <si>
     <t>If a user is associated to the observation unit. For example: a user created a culture. Specifically this is an id from auth_user. Usernames should be used to select this because they are unique.</t>
   </si>
   <si>
@@ -1438,36 +1435,6 @@
     <t>obs_entity_type</t>
   </si>
   <si>
-    <t>A one to one relationship to lab_ObsCulture. Specifically this is the id from lab_ObsCulture. If the obs_entity_type is ObsCulture, then a relevant culture will be recorded here. If the obs_entity_type is not ObsCulture, then obs_culture_id will be 1 and will point to a dummy "No Culture" result. Culture IDs should be used to select this because they are unique.</t>
-  </si>
-  <si>
-    <t>A one to one relationship to lab_ObsDNA. Specifically this is the id from lab_ObsDNA. If the obs_entity_type is ObsDNA, then a relevant record will be here. If the obs_entity_type is not ObsDNA, then obs_dna_id will be 1 and will point to a dummy "No DNA" entry. DNA IDs should be used to select this because they are unique.</t>
-  </si>
-  <si>
-    <t>A one to one relationship to lab_ObsMicrobe. Specifically this is the id from lab_ObsMicrobe. If the obs_entity_type is ObsMicrobe, then a relevant record will be here. If the obs_entity_type is not ObsMicrobe, then obs_microbe_id will be 1 and will point to a dummy "No Microbe" entry. Microbe IDs should be used to select this because they are unique.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A one to one relationship to lab_ObsPlant. Specifically this is the id from lab_ObsPlant. If the obs_entity_type is ObsPlant, then a relevant result will be here. If the obs_entity_type is not ObsPlant, then the obs_plant_id will be 1 and will point to a dummy "No Plant" entry. Plant IDs should be used to select this because they are unique. </t>
-  </si>
-  <si>
-    <t>A one to one relationship to lab_ObsPlate. Specfically this is the id from lab_ObsPlate. If the obs_entity_type is ObsPlate, then a relevant result will be here. If the obs_entity_type is not ObsPlate, then the obs_plate_id will be 1 and will point to a dummy "No Plate" entry. Plate IDs should be used to select this because they are unique.</t>
-  </si>
-  <si>
-    <t>A one to one relationship to lab_ObsRow. Specifically this is the id from lab_ObsRow. If the obs_entity_id is ObsRow, then a relevant result will be here. If the obs_entity_id is not ObsRow, then the obs_row_id will be 1 and will point to a dummy "No Row" entry. Row IDs should be used to select this because they are unique.</t>
-  </si>
-  <si>
-    <t>A one to one relationship to lab_ObsSample. Specifically this is the id from lab_ObsSample. If the obs_entity_id is ObsSample, then a relevant result will be here. If the obs_entity_id is not ObsSample, then the obs_sample_id will be 1 and will point to a dummy "No Sample" entry. Sample IDs should be used to select this because they are unique.</t>
-  </si>
-  <si>
-    <t>A one to one relationship to lab_ObsTissue. Specifically this is the id from lab_ObsTissue. If the obs_entity_id is ObsTissue, then a relevant result will be here. If the obs_entity_id is not ObsTissue, then the obs_tissue_id will be 1 and will point to a dummy "No Tissue" entry. Tissue IDs should be used to select this because they are unique.</t>
-  </si>
-  <si>
-    <t>A one to one relationship to lab_ObsWell. Specifically this is the id from lab_ObsWell. If the obs_entity_id is ObsWell, then a relevant result will be here. If the obs_entity_id is not ObsWell, then the obs_well_id will be 1 and will point to a dummy "No Well" entry. Well IDs should be used to select this because they are unique.</t>
-  </si>
-  <si>
-    <t>A one to one relationship to lab_ObsEnv. Specifically this is the id from lab_ObsEnv. If the obs_entity_id is ObsEnv, then a relevant result will be here. If the obs_entity_id is not ObsEnv, then the obs_env_id will be 1 and will point to a dummy "No Environment" entry. Environment IDs should be used to select this because they are unique.</t>
-  </si>
-  <si>
     <t>lab_ObsTrackerSource</t>
   </si>
   <si>
@@ -1484,6 +1451,200 @@
   </si>
   <si>
     <t>The observation unit that was the source of the target observation unit.</t>
+  </si>
+  <si>
+    <t>A controlled vocab for the type of observation unit being tracked. Either: plant, row, culture, tissue, sample, well, extract, microbe, env, dna, plate, stock, maize, isolate</t>
+  </si>
+  <si>
+    <t>lab_ObsExtract</t>
+  </si>
+  <si>
+    <t>This table holds any extract info that needs to be recorded.</t>
+  </si>
+  <si>
+    <t>extract_id</t>
+  </si>
+  <si>
+    <t>grind_method</t>
+  </si>
+  <si>
+    <t>solvent</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A unique ID for the extract. Formats may vary, but this needs to be unique. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MUST BE UNIQUE</t>
+    </r>
+  </si>
+  <si>
+    <t>The weight of the sample being extracted.</t>
+  </si>
+  <si>
+    <t>The rep number that the extract is a part of.</t>
+  </si>
+  <si>
+    <t>A brief description of the method used to grind the sample. Name any equipment that was used.</t>
+  </si>
+  <si>
+    <t>The kind of solvent used in the extraction. E.G. ethanol, DI water, etc</t>
+  </si>
+  <si>
+    <t>Any additional comments</t>
+  </si>
+  <si>
+    <t>photo</t>
+  </si>
+  <si>
+    <t>The filename of the photo. This is optional.</t>
+  </si>
+  <si>
+    <t>maize_sample_id</t>
+  </si>
+  <si>
+    <t>A link to the observation unit. If this observation unit is not relevant it will be 1, which is a dummy placeholder.</t>
+  </si>
+  <si>
+    <t>If the observation unit is associated with a maize sample. Maize samples are not inventoried seed samples. Maize IDs should be used to select this because they are unique.</t>
+  </si>
+  <si>
+    <t>obs_extract_id</t>
+  </si>
+  <si>
+    <t>lab_MaizeSample</t>
+  </si>
+  <si>
+    <t>This table holds seed info, for seed samples that are not recorded. This is an alternative to the lab_Stock table and is mainly for seed that has minimal info associated with it.</t>
+  </si>
+  <si>
+    <t>A link to the locality from where the maize sample was from, giving city, state, country, zipcode</t>
+  </si>
+  <si>
+    <t>maize_id</t>
+  </si>
+  <si>
+    <t>type_of_source</t>
+  </si>
+  <si>
+    <t>sample_source</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Any additional comments about the maize sample. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A unique ID for the maize sample. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MUST BE UNIQUE</t>
+    </r>
+  </si>
+  <si>
+    <t>A category for the type of source. For example, Market, Mill, Distributor</t>
+  </si>
+  <si>
+    <t>The name of where the maize sample came from. Can be a store name, location, etc.</t>
+  </si>
+  <si>
+    <t>The weight in grams of the maize sample. Can be approximate.</t>
+  </si>
+  <si>
+    <t>A brief description of the maize sample.</t>
+  </si>
+  <si>
+    <t>The photo's filename. Optional</t>
+  </si>
+  <si>
+    <t>lab_Separation</t>
+  </si>
+  <si>
+    <t>If a separation test was done on a sample, it should be recorded here.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A link to the sample that was separated. </t>
+  </si>
+  <si>
+    <t>separation_type</t>
+  </si>
+  <si>
+    <t>apparatus</t>
+  </si>
+  <si>
+    <t>SG</t>
+  </si>
+  <si>
+    <t>light_weight</t>
+  </si>
+  <si>
+    <t>intermediate_weight</t>
+  </si>
+  <si>
+    <t>heavy_weight</t>
+  </si>
+  <si>
+    <t>light_percent</t>
+  </si>
+  <si>
+    <t>intermediate_percent</t>
+  </si>
+  <si>
+    <t>heavy_percent</t>
+  </si>
+  <si>
+    <t>operating_factor</t>
+  </si>
+  <si>
+    <t>Any additional comments about the separation.</t>
+  </si>
+  <si>
+    <t>The type of separation being done. E.G. floatation, air column, gravity table</t>
+  </si>
+  <si>
+    <t>The name of the device being used to separate the sample.</t>
+  </si>
+  <si>
+    <t>The specific gravity for a floatation separation.</t>
+  </si>
+  <si>
+    <t>The weight that was recovered as light.</t>
+  </si>
+  <si>
+    <t>The weight that was recovered as intermediate.</t>
+  </si>
+  <si>
+    <t>The weight that was recovered as heavy.</t>
+  </si>
+  <si>
+    <t>The fraction that was recovered as light.</t>
+  </si>
+  <si>
+    <t>The fraction that was recovered as intermmediate.</t>
+  </si>
+  <si>
+    <t>The fraction that was recovered as heavy.</t>
+  </si>
+  <si>
+    <t>Any operating factor of interest. E.G. 50% power</t>
   </si>
 </sst>
 </file>
@@ -1863,10 +2024,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q315"/>
+  <dimension ref="A1:Q356"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="C187" sqref="C187"/>
+    <sheetView tabSelected="1" topLeftCell="B339" workbookViewId="0">
+      <selection activeCell="C355" sqref="C355"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3115,141 +3276,141 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
+        <v>401</v>
+      </c>
+      <c r="B129" t="s">
+        <v>14</v>
+      </c>
+      <c r="C129" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>5</v>
       </c>
-      <c r="B129" t="s">
-        <v>14</v>
-      </c>
-      <c r="C129" t="s">
+      <c r="B130" t="s">
+        <v>14</v>
+      </c>
+      <c r="C130" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
-      <c r="A131" s="1" t="s">
+    <row r="132" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="A132" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="B131" s="1"/>
-      <c r="C131" s="6" t="s">
+      <c r="B132" s="1"/>
+      <c r="C132" s="6" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A132" s="4" t="s">
+    <row r="133" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A133" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B132" s="4" t="s">
+      <c r="B133" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C132" s="8" t="s">
+      <c r="C133" s="8" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>1</v>
-      </c>
-      <c r="B133" t="s">
-        <v>12</v>
-      </c>
-      <c r="C133" s="7" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>126</v>
+        <v>1</v>
       </c>
       <c r="B134" t="s">
-        <v>14</v>
-      </c>
-      <c r="C134" t="s">
-        <v>147</v>
+        <v>12</v>
+      </c>
+      <c r="C134" s="7" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B135" t="s">
         <v>14</v>
       </c>
       <c r="C135" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B136" t="s">
         <v>14</v>
       </c>
       <c r="C136" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>351</v>
+        <v>128</v>
       </c>
       <c r="B137" t="s">
         <v>14</v>
       </c>
       <c r="C137" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
+        <v>351</v>
+      </c>
+      <c r="B138" t="s">
+        <v>14</v>
+      </c>
+      <c r="C138" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>5</v>
       </c>
-      <c r="B138" t="s">
-        <v>14</v>
-      </c>
-      <c r="C138" t="s">
+      <c r="B139" t="s">
+        <v>14</v>
+      </c>
+      <c r="C139" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
-      <c r="A140" s="1" t="s">
+    <row r="141" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="A141" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="B140" s="1"/>
-      <c r="C140" s="6" t="s">
+      <c r="B141" s="1"/>
+      <c r="C141" s="6" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A141" s="4" t="s">
+    <row r="142" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A142" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B141" s="4" t="s">
+      <c r="B142" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C141" s="8" t="s">
+      <c r="C142" s="8" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>1</v>
-      </c>
-      <c r="B142" t="s">
-        <v>12</v>
-      </c>
-      <c r="C142" s="7" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>135</v>
+        <v>1</v>
       </c>
       <c r="B143" t="s">
-        <v>14</v>
-      </c>
-      <c r="C143" t="s">
-        <v>159</v>
+        <v>12</v>
+      </c>
+      <c r="C143" s="7" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -3260,746 +3421,752 @@
         <v>14</v>
       </c>
       <c r="C144" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B145" t="s">
         <v>14</v>
       </c>
       <c r="C145" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>353</v>
+        <v>136</v>
       </c>
       <c r="B146" t="s">
         <v>14</v>
       </c>
       <c r="C146" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
+        <v>353</v>
+      </c>
+      <c r="B147" t="s">
+        <v>14</v>
+      </c>
+      <c r="C147" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>5</v>
       </c>
-      <c r="B147" t="s">
-        <v>14</v>
-      </c>
-      <c r="C147" t="s">
+      <c r="B148" t="s">
+        <v>14</v>
+      </c>
+      <c r="C148" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
-      <c r="A149" s="1" t="s">
+    <row r="150" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="A150" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="B149" s="1"/>
-      <c r="C149" s="6" t="s">
+      <c r="B150" s="1"/>
+      <c r="C150" s="6" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A150" s="4" t="s">
+    <row r="151" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A151" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B150" s="4" t="s">
+      <c r="B151" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C150" s="8" t="s">
+      <c r="C151" s="8" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>1</v>
-      </c>
-      <c r="B151" t="s">
-        <v>12</v>
-      </c>
-      <c r="C151" s="7" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>129</v>
+        <v>1</v>
       </c>
       <c r="B152" t="s">
-        <v>14</v>
-      </c>
-      <c r="C152" t="s">
-        <v>164</v>
+        <v>12</v>
+      </c>
+      <c r="C152" s="7" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B153" t="s">
         <v>14</v>
       </c>
       <c r="C153" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>23</v>
+        <v>130</v>
       </c>
       <c r="B154" t="s">
         <v>14</v>
       </c>
       <c r="C154" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>355</v>
+        <v>23</v>
       </c>
       <c r="B155" t="s">
         <v>14</v>
       </c>
       <c r="C155" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>91</v>
+        <v>355</v>
       </c>
       <c r="B156" t="s">
         <v>14</v>
       </c>
       <c r="C156" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>131</v>
+        <v>91</v>
       </c>
       <c r="B157" t="s">
         <v>14</v>
       </c>
       <c r="C157" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B158" t="s">
         <v>14</v>
       </c>
       <c r="C158" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
+        <v>132</v>
+      </c>
+      <c r="B159" t="s">
+        <v>14</v>
+      </c>
+      <c r="C159" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>5</v>
       </c>
-      <c r="B159" t="s">
-        <v>14</v>
-      </c>
-      <c r="C159" t="s">
+      <c r="B160" t="s">
+        <v>14</v>
+      </c>
+      <c r="C160" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A161" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="B161" s="1"/>
-      <c r="C161" s="6" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A162" s="4" t="s">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C161"/>
+    </row>
+    <row r="162" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A162" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B162" s="1"/>
+      <c r="C162" s="6" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A163" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B162" s="4" t="s">
+      <c r="B163" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C162" s="8" t="s">
+      <c r="C163" s="8" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>1</v>
-      </c>
-      <c r="B163" t="s">
-        <v>12</v>
-      </c>
-      <c r="C163" s="7" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>383</v>
+        <v>1</v>
       </c>
       <c r="B164" t="s">
-        <v>14</v>
-      </c>
-      <c r="C164" t="s">
-        <v>375</v>
+        <v>12</v>
+      </c>
+      <c r="C164" s="7" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>6</v>
+        <v>392</v>
       </c>
       <c r="B165" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C165" t="s">
-        <v>376</v>
+        <v>395</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>124</v>
+        <v>236</v>
       </c>
       <c r="B166" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C166" t="s">
-        <v>377</v>
+        <v>396</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="B167" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C167" t="s">
-        <v>378</v>
+        <v>397</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>7</v>
+        <v>393</v>
       </c>
       <c r="B168" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C168" t="s">
-        <v>379</v>
+        <v>398</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>247</v>
+        <v>394</v>
       </c>
       <c r="B169" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C169" t="s">
-        <v>380</v>
+        <v>399</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>108</v>
+        <v>5</v>
       </c>
       <c r="B170" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C170" t="s">
-        <v>381</v>
+        <v>400</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>220</v>
-      </c>
-      <c r="B171" t="s">
-        <v>13</v>
-      </c>
-      <c r="C171" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>365</v>
-      </c>
-      <c r="B172" t="s">
-        <v>13</v>
-      </c>
-      <c r="C172" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>366</v>
-      </c>
-      <c r="B173" t="s">
-        <v>13</v>
-      </c>
-      <c r="C173" t="s">
-        <v>385</v>
+      <c r="C171"/>
+    </row>
+    <row r="172" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A172" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B172" s="1"/>
+      <c r="C172" s="6" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A173" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B173" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C173" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>367</v>
+        <v>1</v>
       </c>
       <c r="B174" t="s">
-        <v>13</v>
-      </c>
-      <c r="C174" t="s">
-        <v>386</v>
+        <v>12</v>
+      </c>
+      <c r="C174" s="7" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>368</v>
+        <v>382</v>
       </c>
       <c r="B175" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C175" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>369</v>
+        <v>6</v>
       </c>
       <c r="B176" t="s">
         <v>13</v>
       </c>
       <c r="C176" t="s">
-        <v>388</v>
+        <v>375</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="B177" t="s">
         <v>13</v>
       </c>
       <c r="C177" t="s">
-        <v>389</v>
+        <v>376</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>370</v>
+        <v>20</v>
       </c>
       <c r="B178" t="s">
         <v>13</v>
       </c>
       <c r="C178" t="s">
-        <v>390</v>
+        <v>377</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>371</v>
+        <v>7</v>
       </c>
       <c r="B179" t="s">
         <v>13</v>
       </c>
       <c r="C179" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>372</v>
+        <v>247</v>
       </c>
       <c r="B180" t="s">
         <v>13</v>
       </c>
       <c r="C180" t="s">
-        <v>392</v>
+        <v>379</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>373</v>
+        <v>108</v>
       </c>
       <c r="B181" t="s">
         <v>13</v>
       </c>
       <c r="C181" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C182"/>
-    </row>
-    <row r="183" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A183" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="B183" s="1"/>
-      <c r="C183" s="6" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A184" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B184" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C184" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A185" s="5" t="s">
-        <v>193</v>
+      <c r="A182" t="s">
+        <v>403</v>
+      </c>
+      <c r="B182" t="s">
+        <v>13</v>
+      </c>
+      <c r="C182" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>220</v>
+      </c>
+      <c r="B183" t="s">
+        <v>13</v>
+      </c>
+      <c r="C183" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>365</v>
+      </c>
+      <c r="B184" t="s">
+        <v>13</v>
+      </c>
+      <c r="C184" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>366</v>
       </c>
       <c r="B185" t="s">
-        <v>12</v>
-      </c>
-      <c r="C185" s="7" t="s">
-        <v>279</v>
+        <v>13</v>
+      </c>
+      <c r="C185" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>395</v>
+        <v>367</v>
       </c>
       <c r="B186" t="s">
         <v>13</v>
       </c>
-      <c r="C186" s="7" t="s">
-        <v>397</v>
+      <c r="C186" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>396</v>
+        <v>368</v>
       </c>
       <c r="B187" t="s">
         <v>13</v>
       </c>
-      <c r="C187" s="7" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A189" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="B189" s="1"/>
-      <c r="C189" s="6" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A190" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B190" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C190" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A191" s="5" t="s">
-        <v>193</v>
+      <c r="C187" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>369</v>
+      </c>
+      <c r="B188" t="s">
+        <v>13</v>
+      </c>
+      <c r="C188" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>107</v>
+      </c>
+      <c r="B189" t="s">
+        <v>13</v>
+      </c>
+      <c r="C189" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>370</v>
+      </c>
+      <c r="B190" t="s">
+        <v>13</v>
+      </c>
+      <c r="C190" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>371</v>
       </c>
       <c r="B191" t="s">
-        <v>12</v>
-      </c>
-      <c r="C191" s="7" t="s">
-        <v>279</v>
+        <v>13</v>
+      </c>
+      <c r="C191" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>188</v>
+        <v>372</v>
       </c>
       <c r="B192" t="s">
-        <v>14</v>
-      </c>
-      <c r="C192" s="7" t="s">
-        <v>198</v>
+        <v>13</v>
+      </c>
+      <c r="C192" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>189</v>
+        <v>373</v>
       </c>
       <c r="B193" t="s">
-        <v>14</v>
-      </c>
-      <c r="C193" s="7" t="s">
-        <v>199</v>
+        <v>13</v>
+      </c>
+      <c r="C193" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>190</v>
+        <v>406</v>
       </c>
       <c r="B194" t="s">
-        <v>14</v>
-      </c>
-      <c r="C194" s="7" t="s">
-        <v>202</v>
+        <v>13</v>
+      </c>
+      <c r="C194" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
-        <v>191</v>
-      </c>
-      <c r="B195" t="s">
-        <v>14</v>
-      </c>
-      <c r="C195" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
-        <v>192</v>
-      </c>
-      <c r="B196" t="s">
-        <v>14</v>
-      </c>
-      <c r="C196" s="7" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
-      <c r="A198" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B198" s="1"/>
-      <c r="C198" s="6" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A199" s="4" t="s">
+      <c r="C195"/>
+    </row>
+    <row r="196" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A196" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B196" s="1"/>
+      <c r="C196" s="6" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A197" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B199" s="4" t="s">
+      <c r="B197" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C199" s="8" t="s">
+      <c r="C197" s="8" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A198" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B198" t="s">
+        <v>12</v>
+      </c>
+      <c r="C198" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>384</v>
+      </c>
+      <c r="B199" t="s">
+        <v>13</v>
+      </c>
+      <c r="C199" s="7" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>1</v>
+        <v>385</v>
       </c>
       <c r="B200" t="s">
+        <v>13</v>
+      </c>
+      <c r="C200" s="7" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A202" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B202" s="1"/>
+      <c r="C202" s="6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A203" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B203" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C203" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A204" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B204" t="s">
         <v>12</v>
       </c>
-      <c r="C200" s="7" t="s">
+      <c r="C204" s="7" t="s">
         <v>279</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
-        <v>338</v>
-      </c>
-      <c r="B201" t="s">
-        <v>13</v>
-      </c>
-      <c r="C201" s="7" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
-        <v>194</v>
-      </c>
-      <c r="B202" t="s">
-        <v>13</v>
-      </c>
-      <c r="C202" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
-        <v>6</v>
-      </c>
-      <c r="B203" t="s">
-        <v>13</v>
-      </c>
-      <c r="C203" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
-        <v>195</v>
-      </c>
-      <c r="B204" t="s">
-        <v>14</v>
-      </c>
-      <c r="C204" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B205" t="s">
         <v>14</v>
       </c>
-      <c r="C205" t="s">
-        <v>205</v>
+      <c r="C205" s="7" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>5</v>
+        <v>189</v>
       </c>
       <c r="B206" t="s">
         <v>14</v>
       </c>
-      <c r="C206" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A208" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B208" s="1"/>
-      <c r="C208" s="6" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A209" s="4" t="s">
+      <c r="C206" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>190</v>
+      </c>
+      <c r="B207" t="s">
+        <v>14</v>
+      </c>
+      <c r="C207" s="7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>191</v>
+      </c>
+      <c r="B208" t="s">
+        <v>14</v>
+      </c>
+      <c r="C208" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>192</v>
+      </c>
+      <c r="B209" t="s">
+        <v>14</v>
+      </c>
+      <c r="C209" s="7" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="A211" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B211" s="1"/>
+      <c r="C211" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A212" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B209" s="4" t="s">
+      <c r="B212" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C209" s="8" t="s">
+      <c r="C212" s="8" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
-        <v>1</v>
-      </c>
-      <c r="B210" t="s">
-        <v>12</v>
-      </c>
-      <c r="C210" s="7" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
-        <v>218</v>
-      </c>
-      <c r="B211" t="s">
-        <v>13</v>
-      </c>
-      <c r="C211" s="7" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
-        <v>211</v>
-      </c>
-      <c r="B212" t="s">
-        <v>14</v>
-      </c>
-      <c r="C212" s="7" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>212</v>
+        <v>1</v>
       </c>
       <c r="B213" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C213" s="7" t="s">
-        <v>254</v>
+        <v>279</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>213</v>
+        <v>338</v>
       </c>
       <c r="B214" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C214" s="7" t="s">
-        <v>255</v>
+        <v>339</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="B215" t="s">
-        <v>14</v>
-      </c>
-      <c r="C215" s="7" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="C215" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>215</v>
+        <v>6</v>
       </c>
       <c r="B216" t="s">
-        <v>14</v>
-      </c>
-      <c r="C216" s="7" t="s">
-        <v>257</v>
+        <v>13</v>
+      </c>
+      <c r="C216" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="B217" t="s">
         <v>14</v>
       </c>
-      <c r="C217" s="7" t="s">
-        <v>258</v>
+      <c r="C217" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="B218" t="s">
         <v>14</v>
       </c>
-      <c r="C218" s="7" t="s">
-        <v>259</v>
+      <c r="C218" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
@@ -4009,17 +4176,20 @@
       <c r="B219" t="s">
         <v>14</v>
       </c>
-      <c r="C219" s="7" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="221" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="C219" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C220"/>
+    </row>
+    <row r="221" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A221" s="1" t="s">
-        <v>219</v>
+        <v>407</v>
       </c>
       <c r="B221" s="1"/>
       <c r="C221" s="6" t="s">
-        <v>264</v>
+        <v>408</v>
       </c>
     </row>
     <row r="222" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4044,902 +4214,1314 @@
         <v>279</v>
       </c>
     </row>
-    <row r="224" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>220</v>
+        <v>34</v>
       </c>
       <c r="B224" t="s">
         <v>13</v>
       </c>
       <c r="C224" s="7" t="s">
-        <v>265</v>
+        <v>409</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>221</v>
+        <v>410</v>
       </c>
       <c r="B225" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C225" s="7" t="s">
-        <v>261</v>
+        <v>415</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>222</v>
+        <v>411</v>
       </c>
       <c r="B226" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C226" s="7" t="s">
-        <v>262</v>
+        <v>416</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C227"/>
-    </row>
-    <row r="228" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
-      <c r="A228" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="B228" s="1"/>
-      <c r="C228" s="6" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A229" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B229" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C229" s="8" t="s">
-        <v>11</v>
+      <c r="A227" t="s">
+        <v>412</v>
+      </c>
+      <c r="B227" t="s">
+        <v>14</v>
+      </c>
+      <c r="C227" s="7" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>236</v>
+      </c>
+      <c r="B228" t="s">
+        <v>14</v>
+      </c>
+      <c r="C228" s="7" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>413</v>
+      </c>
+      <c r="B229" t="s">
+        <v>14</v>
+      </c>
+      <c r="C229" s="7" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>1</v>
+        <v>401</v>
       </c>
       <c r="B230" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C230" s="7" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>85</v>
+        <v>5</v>
       </c>
       <c r="B231" t="s">
-        <v>13</v>
-      </c>
-      <c r="C231" s="7" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A232" t="s">
-        <v>7</v>
-      </c>
-      <c r="B232" t="s">
-        <v>13</v>
-      </c>
-      <c r="C232" s="7" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A233" t="s">
-        <v>6</v>
-      </c>
-      <c r="B233" t="s">
-        <v>13</v>
-      </c>
-      <c r="C233" s="7" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A234" t="s">
-        <v>224</v>
-      </c>
-      <c r="B234" t="s">
-        <v>14</v>
-      </c>
-      <c r="C234" s="7" t="s">
-        <v>269</v>
+        <v>14</v>
+      </c>
+      <c r="C231" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A233" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B233" s="1"/>
+      <c r="C233" s="6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A234" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B234" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C234" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>225</v>
+        <v>1</v>
       </c>
       <c r="B235" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C235" s="7" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>5</v>
+        <v>218</v>
       </c>
       <c r="B236" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C236" s="7" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
-      <c r="A238" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B238" s="1"/>
-      <c r="C238" s="6" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A239" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B239" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C239" s="8" t="s">
-        <v>11</v>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>211</v>
+      </c>
+      <c r="B237" t="s">
+        <v>14</v>
+      </c>
+      <c r="C237" s="7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>212</v>
+      </c>
+      <c r="B238" t="s">
+        <v>14</v>
+      </c>
+      <c r="C238" s="7" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>213</v>
+      </c>
+      <c r="B239" t="s">
+        <v>14</v>
+      </c>
+      <c r="C239" s="7" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>1</v>
+        <v>214</v>
       </c>
       <c r="B240" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C240" s="7" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>53</v>
+        <v>215</v>
       </c>
       <c r="B241" t="s">
         <v>14</v>
       </c>
       <c r="C241" s="7" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>54</v>
+        <v>216</v>
       </c>
       <c r="B242" t="s">
         <v>14</v>
       </c>
       <c r="C242" s="7" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>73</v>
+        <v>217</v>
       </c>
       <c r="B243" t="s">
         <v>14</v>
       </c>
       <c r="C243" s="7" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>71</v>
+        <v>5</v>
       </c>
       <c r="B244" t="s">
         <v>14</v>
       </c>
       <c r="C244" s="7" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A245" t="s">
-        <v>55</v>
-      </c>
-      <c r="B245" t="s">
-        <v>14</v>
-      </c>
-      <c r="C245" s="7" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A246" t="s">
-        <v>5</v>
-      </c>
-      <c r="B246" t="s">
-        <v>14</v>
-      </c>
-      <c r="C246" s="7" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="248" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A248" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="B248" s="1"/>
-      <c r="C248" s="6" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A249" s="4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A246" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B246" s="1"/>
+      <c r="C246" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A247" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B249" s="4" t="s">
+      <c r="B247" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C249" s="8" t="s">
+      <c r="C247" s="8" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>1</v>
+      </c>
+      <c r="B248" t="s">
+        <v>12</v>
+      </c>
+      <c r="C248" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>220</v>
+      </c>
+      <c r="B249" t="s">
+        <v>13</v>
+      </c>
+      <c r="C249" s="7" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>1</v>
+        <v>221</v>
       </c>
       <c r="B250" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C250" s="7" t="s">
-        <v>279</v>
+        <v>261</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B251" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C251" s="7" t="s">
-        <v>285</v>
+        <v>262</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A252" t="s">
-        <v>229</v>
-      </c>
-      <c r="B252" t="s">
-        <v>14</v>
-      </c>
-      <c r="C252" s="7" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A253" t="s">
-        <v>230</v>
-      </c>
-      <c r="B253" t="s">
-        <v>14</v>
-      </c>
-      <c r="C253" s="7" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A254" t="s">
-        <v>231</v>
-      </c>
-      <c r="B254" t="s">
-        <v>14</v>
-      </c>
-      <c r="C254" s="7" t="s">
-        <v>281</v>
+      <c r="C252"/>
+    </row>
+    <row r="253" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="A253" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B253" s="1"/>
+      <c r="C253" s="6" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A254" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B254" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C254" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>232</v>
+        <v>1</v>
       </c>
       <c r="B255" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C255" s="7" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>233</v>
+        <v>85</v>
       </c>
       <c r="B256" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C256" s="7" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>234</v>
+        <v>7</v>
       </c>
       <c r="B257" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C257" s="7" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="259" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
-      <c r="A259" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B259" s="1"/>
-      <c r="C259" s="6" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="260" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A260" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B260" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C260" s="8" t="s">
-        <v>11</v>
+        <v>267</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>6</v>
+      </c>
+      <c r="B258" t="s">
+        <v>13</v>
+      </c>
+      <c r="C258" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>224</v>
+      </c>
+      <c r="B259" t="s">
+        <v>14</v>
+      </c>
+      <c r="C259" s="7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>225</v>
+      </c>
+      <c r="B260" t="s">
+        <v>14</v>
+      </c>
+      <c r="C260" s="7" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B261" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C261" s="7" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A262" t="s">
-        <v>108</v>
-      </c>
-      <c r="B262" t="s">
-        <v>13</v>
-      </c>
-      <c r="C262" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="263" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A263" t="s">
-        <v>124</v>
-      </c>
-      <c r="B263" t="s">
-        <v>13</v>
-      </c>
-      <c r="C263" s="7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A264" t="s">
-        <v>236</v>
-      </c>
-      <c r="B264" t="s">
-        <v>14</v>
-      </c>
-      <c r="C264" s="7" t="s">
-        <v>291</v>
+        <v>271</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="A263" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B263" s="1"/>
+      <c r="C263" s="6" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A264" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B264" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C264" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>237</v>
+        <v>1</v>
       </c>
       <c r="B265" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C265" s="7" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="B266" t="s">
         <v>14</v>
       </c>
       <c r="C266" s="7" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="268" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A268" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="B268" s="1"/>
-      <c r="C268" s="6" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="269" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A269" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B269" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C269" s="8" t="s">
-        <v>11</v>
+        <v>273</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>54</v>
+      </c>
+      <c r="B267" t="s">
+        <v>14</v>
+      </c>
+      <c r="C267" s="7" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>73</v>
+      </c>
+      <c r="B268" t="s">
+        <v>14</v>
+      </c>
+      <c r="C268" s="7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>71</v>
+      </c>
+      <c r="B269" t="s">
+        <v>14</v>
+      </c>
+      <c r="C269" s="7" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B270" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C270" s="7" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="B271" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C271" s="7" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A272" t="s">
-        <v>240</v>
-      </c>
-      <c r="B272" t="s">
-        <v>14</v>
-      </c>
-      <c r="C272" s="3" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A273" t="s">
-        <v>239</v>
-      </c>
-      <c r="B273" t="s">
-        <v>14</v>
-      </c>
-      <c r="C273" s="3" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A274" t="s">
-        <v>241</v>
-      </c>
-      <c r="B274" t="s">
-        <v>14</v>
-      </c>
-      <c r="C274" s="3" t="s">
-        <v>297</v>
+        <v>278</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A273" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B273" s="1"/>
+      <c r="C273" s="6" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A274" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B274" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C274" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>242</v>
+        <v>1</v>
       </c>
       <c r="B275" t="s">
-        <v>14</v>
-      </c>
-      <c r="C275" s="3" t="s">
-        <v>298</v>
+        <v>12</v>
+      </c>
+      <c r="C275" s="7" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="B276" t="s">
         <v>14</v>
       </c>
-      <c r="C276" s="3" t="s">
-        <v>299</v>
+      <c r="C276" s="7" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="B277" t="s">
         <v>14</v>
       </c>
-      <c r="C277" s="3" t="s">
-        <v>300</v>
+      <c r="C277" s="7" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>5</v>
+        <v>230</v>
       </c>
       <c r="B278" t="s">
         <v>14</v>
       </c>
-      <c r="C278" s="3" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A280" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="B280" s="1"/>
-      <c r="C280" s="6" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="281" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A281" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B281" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C281" s="8" t="s">
-        <v>11</v>
+      <c r="C278" s="7" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>231</v>
+      </c>
+      <c r="B279" t="s">
+        <v>14</v>
+      </c>
+      <c r="C279" s="7" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>232</v>
+      </c>
+      <c r="B280" t="s">
+        <v>14</v>
+      </c>
+      <c r="C280" s="7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>233</v>
+      </c>
+      <c r="B281" t="s">
+        <v>14</v>
+      </c>
+      <c r="C281" s="7" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>1</v>
+        <v>234</v>
       </c>
       <c r="B282" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C282" s="7" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A283" t="s">
-        <v>218</v>
-      </c>
-      <c r="B283" t="s">
-        <v>13</v>
-      </c>
-      <c r="C283" s="7" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="284" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A284" t="s">
-        <v>124</v>
-      </c>
-      <c r="B284" t="s">
-        <v>13</v>
-      </c>
-      <c r="C284" s="7" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A285" t="s">
-        <v>246</v>
-      </c>
-      <c r="B285" t="s">
-        <v>13</v>
-      </c>
-      <c r="C285" s="7" t="s">
-        <v>305</v>
+        <v>284</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="A284" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B284" s="1"/>
+      <c r="C284" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A285" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B285" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C285" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>247</v>
+        <v>1</v>
       </c>
       <c r="B286" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C286" s="7" t="s">
-        <v>306</v>
+        <v>279</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>248</v>
+        <v>108</v>
       </c>
       <c r="B287" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C287" s="7" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>249</v>
+        <v>124</v>
       </c>
       <c r="B288" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C288" s="7" t="s">
-        <v>308</v>
+        <v>290</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
+        <v>236</v>
+      </c>
+      <c r="B289" t="s">
+        <v>14</v>
+      </c>
+      <c r="C289" s="7" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>237</v>
+      </c>
+      <c r="B290" t="s">
+        <v>14</v>
+      </c>
+      <c r="C290" s="7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
         <v>5</v>
       </c>
-      <c r="B289" t="s">
-        <v>14</v>
-      </c>
-      <c r="C289" s="7" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="291" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A291" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="B291" s="1"/>
-      <c r="C291" s="6" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="292" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A292" s="4" t="s">
+      <c r="B291" t="s">
+        <v>14</v>
+      </c>
+      <c r="C291" s="7" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A293" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B293" s="1"/>
+      <c r="C293" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A294" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B292" s="4" t="s">
+      <c r="B294" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C292" s="8" t="s">
+      <c r="C294" s="8" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A293" t="s">
-        <v>1</v>
-      </c>
-      <c r="B293" t="s">
-        <v>12</v>
-      </c>
-      <c r="C293" s="7" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A294" t="s">
-        <v>231</v>
-      </c>
-      <c r="B294" t="s">
-        <v>14</v>
-      </c>
-      <c r="C294" s="7" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>251</v>
+        <v>1</v>
       </c>
       <c r="B295" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C295" s="7" t="s">
-        <v>312</v>
+        <v>279</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B296" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C296" s="7" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="298" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A298" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="B298" s="1"/>
-      <c r="C298" s="6" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="299" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A299" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B299" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C299" s="8" t="s">
-        <v>11</v>
+        <v>295</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>240</v>
+      </c>
+      <c r="B297" t="s">
+        <v>14</v>
+      </c>
+      <c r="C297" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>239</v>
+      </c>
+      <c r="B298" t="s">
+        <v>14</v>
+      </c>
+      <c r="C298" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>241</v>
+      </c>
+      <c r="B299" t="s">
+        <v>14</v>
+      </c>
+      <c r="C299" s="3" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>1</v>
+        <v>242</v>
       </c>
       <c r="B300" t="s">
-        <v>12</v>
-      </c>
-      <c r="C300" s="7" t="s">
-        <v>279</v>
+        <v>14</v>
+      </c>
+      <c r="C300" s="3" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>322</v>
+        <v>243</v>
       </c>
       <c r="B301" t="s">
         <v>14</v>
       </c>
-      <c r="C301" s="7" t="s">
-        <v>323</v>
+      <c r="C301" s="3" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>317</v>
+        <v>244</v>
       </c>
       <c r="B302" t="s">
         <v>14</v>
       </c>
-      <c r="C302" s="7" t="s">
-        <v>320</v>
+      <c r="C302" s="3" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>318</v>
+        <v>5</v>
       </c>
       <c r="B303" t="s">
         <v>14</v>
       </c>
-      <c r="C303" s="7" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A304" t="s">
-        <v>319</v>
-      </c>
-      <c r="B304" t="s">
-        <v>14</v>
-      </c>
-      <c r="C304" s="7" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A305" t="s">
-        <v>5</v>
-      </c>
-      <c r="B305" t="s">
-        <v>14</v>
-      </c>
-      <c r="C305" s="7" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="307" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A307" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="B307" s="1"/>
-      <c r="C307" s="6" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="308" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A308" s="4" t="s">
+      <c r="C303" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A305" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B305" s="1"/>
+      <c r="C305" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A306" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B308" s="4" t="s">
+      <c r="B306" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C308" s="8" t="s">
+      <c r="C306" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>1</v>
+      </c>
+      <c r="B307" t="s">
+        <v>12</v>
+      </c>
+      <c r="C307" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>218</v>
+      </c>
+      <c r="B308" t="s">
+        <v>13</v>
+      </c>
+      <c r="C308" s="7" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>1</v>
+        <v>124</v>
       </c>
       <c r="B309" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C309" s="7" t="s">
-        <v>279</v>
+        <v>304</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>317</v>
+        <v>246</v>
       </c>
       <c r="B310" t="s">
         <v>13</v>
       </c>
       <c r="C310" s="7" t="s">
-        <v>332</v>
+        <v>305</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>328</v>
+        <v>247</v>
       </c>
       <c r="B311" t="s">
         <v>14</v>
       </c>
       <c r="C311" s="7" t="s">
-        <v>333</v>
+        <v>306</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>329</v>
+        <v>248</v>
       </c>
       <c r="B312" t="s">
         <v>14</v>
       </c>
       <c r="C312" s="7" t="s">
-        <v>334</v>
+        <v>307</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>330</v>
+        <v>249</v>
       </c>
       <c r="B313" t="s">
         <v>14</v>
       </c>
       <c r="C313" s="7" t="s">
-        <v>335</v>
+        <v>308</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
+        <v>5</v>
+      </c>
+      <c r="B314" t="s">
+        <v>14</v>
+      </c>
+      <c r="C314" s="7" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A316" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B316" s="1"/>
+      <c r="C316" s="6" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A317" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B317" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C317" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>1</v>
+      </c>
+      <c r="B318" t="s">
+        <v>12</v>
+      </c>
+      <c r="C318" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>231</v>
+      </c>
+      <c r="B319" t="s">
+        <v>14</v>
+      </c>
+      <c r="C319" s="7" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>251</v>
+      </c>
+      <c r="B320" t="s">
+        <v>14</v>
+      </c>
+      <c r="C320" s="7" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>5</v>
+      </c>
+      <c r="B321" t="s">
+        <v>14</v>
+      </c>
+      <c r="C321" s="7" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A323" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B323" s="1"/>
+      <c r="C323" s="6" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A324" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B324" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C324" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>1</v>
+      </c>
+      <c r="B325" t="s">
+        <v>12</v>
+      </c>
+      <c r="C325" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>322</v>
+      </c>
+      <c r="B326" t="s">
+        <v>14</v>
+      </c>
+      <c r="C326" s="7" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>317</v>
+      </c>
+      <c r="B327" t="s">
+        <v>14</v>
+      </c>
+      <c r="C327" s="7" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>318</v>
+      </c>
+      <c r="B328" t="s">
+        <v>14</v>
+      </c>
+      <c r="C328" s="7" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>319</v>
+      </c>
+      <c r="B329" t="s">
+        <v>14</v>
+      </c>
+      <c r="C329" s="7" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>5</v>
+      </c>
+      <c r="B330" t="s">
+        <v>14</v>
+      </c>
+      <c r="C330" s="7" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A332" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B332" s="1"/>
+      <c r="C332" s="6" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A333" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B333" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C333" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>1</v>
+      </c>
+      <c r="B334" t="s">
+        <v>12</v>
+      </c>
+      <c r="C334" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>317</v>
+      </c>
+      <c r="B335" t="s">
+        <v>13</v>
+      </c>
+      <c r="C335" s="7" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>328</v>
+      </c>
+      <c r="B336" t="s">
+        <v>14</v>
+      </c>
+      <c r="C336" s="7" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>329</v>
+      </c>
+      <c r="B337" t="s">
+        <v>14</v>
+      </c>
+      <c r="C337" s="7" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>330</v>
+      </c>
+      <c r="B338" t="s">
+        <v>14</v>
+      </c>
+      <c r="C338" s="7" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
         <v>331</v>
       </c>
-      <c r="B314" t="s">
-        <v>14</v>
-      </c>
-      <c r="C314" s="7" t="s">
+      <c r="B339" t="s">
+        <v>14</v>
+      </c>
+      <c r="C339" s="7" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A315" t="s">
+    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
         <v>5</v>
       </c>
-      <c r="B315" t="s">
-        <v>14</v>
-      </c>
-      <c r="C315" s="7" t="s">
+      <c r="B340" t="s">
+        <v>14</v>
+      </c>
+      <c r="C340" s="7" t="s">
         <v>337</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A342" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B342" s="1"/>
+      <c r="C342" s="6" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A343" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B343" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C343" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>1</v>
+      </c>
+      <c r="B344" t="s">
+        <v>12</v>
+      </c>
+      <c r="C344" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>370</v>
+      </c>
+      <c r="B345" t="s">
+        <v>13</v>
+      </c>
+      <c r="C345" s="7" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>424</v>
+      </c>
+      <c r="B346" t="s">
+        <v>14</v>
+      </c>
+      <c r="C346" s="7" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>425</v>
+      </c>
+      <c r="B347" t="s">
+        <v>14</v>
+      </c>
+      <c r="C347" s="7" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
+        <v>426</v>
+      </c>
+      <c r="B348" t="s">
+        <v>14</v>
+      </c>
+      <c r="C348" s="7" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>427</v>
+      </c>
+      <c r="B349" t="s">
+        <v>14</v>
+      </c>
+      <c r="C349" s="7" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>428</v>
+      </c>
+      <c r="B350" t="s">
+        <v>14</v>
+      </c>
+      <c r="C350" s="7" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>429</v>
+      </c>
+      <c r="B351" t="s">
+        <v>14</v>
+      </c>
+      <c r="C351" s="7" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>430</v>
+      </c>
+      <c r="B352" t="s">
+        <v>14</v>
+      </c>
+      <c r="C352" s="7" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>431</v>
+      </c>
+      <c r="B353" t="s">
+        <v>14</v>
+      </c>
+      <c r="C353" s="7" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
+        <v>432</v>
+      </c>
+      <c r="B354" t="s">
+        <v>14</v>
+      </c>
+      <c r="C354" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>433</v>
+      </c>
+      <c r="B355" t="s">
+        <v>14</v>
+      </c>
+      <c r="C355" s="7" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>5</v>
+      </c>
+      <c r="B356" t="s">
+        <v>14</v>
+      </c>
+      <c r="C356" s="7" t="s">
+        <v>434</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added online form interface for editing and adding seed and seed inventory
</commit_message>
<xml_diff>
--- a/NelsonLab Online Database Dictionary.xlsx
+++ b/NelsonLab Online Database Dictionary.xlsx
@@ -1140,22 +1140,6 @@
     <t xml:space="preserve">Any additional comments about the location of the culture. </t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">A descriptive and unique name for the location. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>MUST BE UNIQUE</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">The passport gives details about where the isolate came from and exactly what the isolate is. Specifically this is an id from lab_isolate. </t>
   </si>
   <si>
@@ -1645,6 +1629,9 @@
   </si>
   <si>
     <t>Any operating factor of interest. E.G. 50% power</t>
+  </si>
+  <si>
+    <t>A descriptive name for the location.</t>
   </si>
 </sst>
 </file>
@@ -2026,8 +2013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q356"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B339" workbookViewId="0">
-      <selection activeCell="C355" sqref="C355"/>
+    <sheetView tabSelected="1" topLeftCell="A285" workbookViewId="0">
+      <selection activeCell="C300" sqref="C300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2921,11 +2908,11 @@
     </row>
     <row r="93" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B93" s="1"/>
       <c r="C93" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2963,7 +2950,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B97" t="s">
         <v>14</v>
@@ -2985,7 +2972,7 @@
     </row>
     <row r="99" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B99" t="s">
         <v>14</v>
@@ -2996,7 +2983,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B100" t="s">
         <v>14</v>
@@ -3018,11 +3005,11 @@
     </row>
     <row r="103" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B103" s="1"/>
       <c r="C103" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -3082,11 +3069,11 @@
     </row>
     <row r="110" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B110" s="1"/>
       <c r="C110" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -3119,7 +3106,7 @@
         <v>13</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -3157,7 +3144,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B117" t="s">
         <v>14</v>
@@ -3168,7 +3155,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B118" t="s">
         <v>14</v>
@@ -3179,7 +3166,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B119" t="s">
         <v>14</v>
@@ -3201,11 +3188,11 @@
     </row>
     <row r="122" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B122" s="1"/>
       <c r="C122" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -3276,13 +3263,13 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
+        <v>400</v>
+      </c>
+      <c r="B129" t="s">
+        <v>14</v>
+      </c>
+      <c r="C129" t="s">
         <v>401</v>
-      </c>
-      <c r="B129" t="s">
-        <v>14</v>
-      </c>
-      <c r="C129" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -3298,11 +3285,11 @@
     </row>
     <row r="132" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B132" s="1"/>
       <c r="C132" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -3362,7 +3349,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B138" t="s">
         <v>14</v>
@@ -3384,11 +3371,11 @@
     </row>
     <row r="141" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B141" s="1"/>
       <c r="C141" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -3448,7 +3435,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B147" t="s">
         <v>14</v>
@@ -3470,11 +3457,11 @@
     </row>
     <row r="150" spans="1:3" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B150" s="1"/>
       <c r="C150" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -3534,7 +3521,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B156" t="s">
         <v>14</v>
@@ -3592,11 +3579,11 @@
     </row>
     <row r="162" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B162" s="1"/>
       <c r="C162" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -3623,13 +3610,13 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B165" t="s">
         <v>14</v>
       </c>
       <c r="C165" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -3640,7 +3627,7 @@
         <v>14</v>
       </c>
       <c r="C166" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -3651,29 +3638,29 @@
         <v>14</v>
       </c>
       <c r="C167" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B168" t="s">
         <v>14</v>
       </c>
       <c r="C168" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B169" t="s">
         <v>14</v>
       </c>
       <c r="C169" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -3684,7 +3671,7 @@
         <v>14</v>
       </c>
       <c r="C170" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -3692,11 +3679,11 @@
     </row>
     <row r="172" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B172" s="1"/>
       <c r="C172" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -3723,13 +3710,13 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B175" t="s">
         <v>14</v>
       </c>
       <c r="C175" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -3740,7 +3727,7 @@
         <v>13</v>
       </c>
       <c r="C176" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -3751,7 +3738,7 @@
         <v>13</v>
       </c>
       <c r="C177" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -3762,7 +3749,7 @@
         <v>13</v>
       </c>
       <c r="C178" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -3773,7 +3760,7 @@
         <v>13</v>
       </c>
       <c r="C179" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -3784,7 +3771,7 @@
         <v>13</v>
       </c>
       <c r="C180" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -3795,18 +3782,18 @@
         <v>13</v>
       </c>
       <c r="C181" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B182" t="s">
         <v>13</v>
       </c>
       <c r="C182" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -3817,62 +3804,62 @@
         <v>13</v>
       </c>
       <c r="C183" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B184" t="s">
         <v>13</v>
       </c>
       <c r="C184" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B185" t="s">
         <v>13</v>
       </c>
       <c r="C185" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B186" t="s">
         <v>13</v>
       </c>
       <c r="C186" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B187" t="s">
         <v>13</v>
       </c>
       <c r="C187" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B188" t="s">
         <v>13</v>
       </c>
       <c r="C188" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
@@ -3883,62 +3870,62 @@
         <v>13</v>
       </c>
       <c r="C189" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B190" t="s">
         <v>13</v>
       </c>
       <c r="C190" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B191" t="s">
         <v>13</v>
       </c>
       <c r="C191" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B192" t="s">
         <v>13</v>
       </c>
       <c r="C192" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B193" t="s">
         <v>13</v>
       </c>
       <c r="C193" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B194" t="s">
         <v>13</v>
       </c>
       <c r="C194" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -3946,11 +3933,11 @@
     </row>
     <row r="196" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A196" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B196" s="1"/>
       <c r="C196" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="197" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -3977,24 +3964,24 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B199" t="s">
         <v>13</v>
       </c>
       <c r="C199" s="7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B200" t="s">
         <v>13</v>
       </c>
       <c r="C200" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="21" x14ac:dyDescent="0.35">
@@ -4116,13 +4103,13 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B214" t="s">
         <v>13</v>
       </c>
       <c r="C214" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
@@ -4185,11 +4172,11 @@
     </row>
     <row r="221" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A221" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B221" s="1"/>
       <c r="C221" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="222" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4222,40 +4209,40 @@
         <v>13</v>
       </c>
       <c r="C224" s="7" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B225" t="s">
         <v>14</v>
       </c>
       <c r="C225" s="7" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B226" t="s">
         <v>14</v>
       </c>
       <c r="C226" s="7" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B227" t="s">
         <v>14</v>
       </c>
       <c r="C227" s="7" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
@@ -4266,29 +4253,29 @@
         <v>14</v>
       </c>
       <c r="C228" s="7" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B229" t="s">
         <v>14</v>
       </c>
       <c r="C229" s="7" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B230" t="s">
         <v>14</v>
       </c>
       <c r="C230" s="7" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
@@ -4299,7 +4286,7 @@
         <v>14</v>
       </c>
       <c r="C231" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="233" spans="1:3" ht="21" x14ac:dyDescent="0.35">
@@ -4937,7 +4924,7 @@
         <v>14</v>
       </c>
       <c r="C297" s="3" t="s">
-        <v>302</v>
+        <v>444</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
@@ -5012,7 +4999,7 @@
       </c>
       <c r="B305" s="1"/>
       <c r="C305" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="306" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -5045,7 +5032,7 @@
         <v>13</v>
       </c>
       <c r="C308" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="309" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -5056,7 +5043,7 @@
         <v>13</v>
       </c>
       <c r="C309" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
@@ -5067,7 +5054,7 @@
         <v>13</v>
       </c>
       <c r="C310" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
@@ -5078,7 +5065,7 @@
         <v>14</v>
       </c>
       <c r="C311" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
@@ -5089,7 +5076,7 @@
         <v>14</v>
       </c>
       <c r="C312" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
@@ -5100,7 +5087,7 @@
         <v>14</v>
       </c>
       <c r="C313" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
@@ -5111,7 +5098,7 @@
         <v>14</v>
       </c>
       <c r="C314" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="316" spans="1:3" ht="21" x14ac:dyDescent="0.35">
@@ -5120,7 +5107,7 @@
       </c>
       <c r="B316" s="1"/>
       <c r="C316" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="317" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -5153,7 +5140,7 @@
         <v>14</v>
       </c>
       <c r="C319" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
@@ -5164,7 +5151,7 @@
         <v>14</v>
       </c>
       <c r="C320" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
@@ -5175,16 +5162,16 @@
         <v>14</v>
       </c>
       <c r="C321" s="7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="323" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A323" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B323" s="1"/>
       <c r="C323" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="324" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -5211,46 +5198,46 @@
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
+        <v>321</v>
+      </c>
+      <c r="B326" t="s">
+        <v>14</v>
+      </c>
+      <c r="C326" s="7" t="s">
         <v>322</v>
-      </c>
-      <c r="B326" t="s">
-        <v>14</v>
-      </c>
-      <c r="C326" s="7" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B327" t="s">
         <v>14</v>
       </c>
       <c r="C327" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B328" t="s">
         <v>14</v>
       </c>
       <c r="C328" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B329" t="s">
         <v>14</v>
       </c>
       <c r="C329" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.25">
@@ -5261,16 +5248,16 @@
         <v>14</v>
       </c>
       <c r="C330" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="332" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A332" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B332" s="1"/>
       <c r="C332" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="333" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -5297,57 +5284,57 @@
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B335" t="s">
         <v>13</v>
       </c>
       <c r="C335" s="7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B336" t="s">
         <v>14</v>
       </c>
       <c r="C336" s="7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B337" t="s">
         <v>14</v>
       </c>
       <c r="C337" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B338" t="s">
         <v>14</v>
       </c>
       <c r="C338" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B339" t="s">
         <v>14</v>
       </c>
       <c r="C339" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.25">
@@ -5358,16 +5345,16 @@
         <v>14</v>
       </c>
       <c r="C340" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="342" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A342" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B342" s="1"/>
       <c r="C342" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="343" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -5394,123 +5381,123 @@
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B345" t="s">
         <v>13</v>
       </c>
       <c r="C345" s="7" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B346" t="s">
         <v>14</v>
       </c>
       <c r="C346" s="7" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B347" t="s">
         <v>14</v>
       </c>
       <c r="C347" s="7" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B348" t="s">
         <v>14</v>
       </c>
       <c r="C348" s="7" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B349" t="s">
         <v>14</v>
       </c>
       <c r="C349" s="7" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B350" t="s">
         <v>14</v>
       </c>
       <c r="C350" s="7" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B351" t="s">
         <v>14</v>
       </c>
       <c r="C351" s="7" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B352" t="s">
         <v>14</v>
       </c>
       <c r="C352" s="7" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B353" t="s">
         <v>14</v>
       </c>
       <c r="C353" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B354" t="s">
         <v>14</v>
       </c>
       <c r="C354" s="7" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B355" t="s">
         <v>14</v>
       </c>
       <c r="C355" s="7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.25">
@@ -5521,7 +5508,7 @@
         <v>14</v>
       </c>
       <c r="C356" s="7" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
   </sheetData>

</xml_diff>